<commit_message>
Update LibraireCourriel.cs + validations champs, Add page modif profil vendeur
</commit_message>
<xml_diff>
--- a/Jeu d'essai.xlsx
+++ b/Jeu d'essai.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="125" documentId="114_{8D9B191C-2013-4270-87A9-3FB899E57325}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{46D0E170-26AA-4533-9861-720691A4CABD}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="114_{8D9B191C-2013-4270-87A9-3FB899E57325}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{4DE29F17-CD87-41D4-A643-08A4CC30A177}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PPVendeurs" sheetId="13" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="790">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="789">
   <si>
     <t>NULL</t>
   </si>
@@ -2259,9 +2259,6 @@
     <t>ppuces@gmail.com</t>
   </si>
   <si>
-    <t>Secret98112</t>
-  </si>
-  <si>
     <t>203.99</t>
   </si>
   <si>
@@ -2370,27 +2367,6 @@
     <t>15.00</t>
   </si>
   <si>
-    <t>vendeur11@gmail.com</t>
-  </si>
-  <si>
-    <t>vendeur12@gmail.com</t>
-  </si>
-  <si>
-    <t>vendeur13@gmail.com</t>
-  </si>
-  <si>
-    <t>vendeur14@gmail.com</t>
-  </si>
-  <si>
-    <t>vendeur15@gmail.com</t>
-  </si>
-  <si>
-    <t>vendeur16@gmail.com</t>
-  </si>
-  <si>
-    <t>vendeur17@gmail.com</t>
-  </si>
-  <si>
     <t>Secret123</t>
   </si>
   <si>
@@ -2464,6 +2440,27 @@
   </si>
   <si>
     <t>K0H1Y0</t>
+  </si>
+  <si>
+    <t>vendeur11@outlook.com</t>
+  </si>
+  <si>
+    <t>vendeur12@outlook.com</t>
+  </si>
+  <si>
+    <t>vendeur13@outlook.com</t>
+  </si>
+  <si>
+    <t>vendeur14@outlook.com</t>
+  </si>
+  <si>
+    <t>vendeur15@outlook.com</t>
+  </si>
+  <si>
+    <t>vendeur16@outlook.com</t>
+  </si>
+  <si>
+    <t>vendeur17@outlook.com</t>
   </si>
 </sst>
 </file>
@@ -2801,30 +2798,30 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2889,7 +2886,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11</v>
       </c>
@@ -2924,10 +2921,10 @@
         <v>0</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>758</v>
+        <v>782</v>
       </c>
       <c r="M2" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="N2">
         <v>500</v>
@@ -2954,7 +2951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>12</v>
       </c>
@@ -2989,10 +2986,10 @@
         <v>0</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>759</v>
+        <v>783</v>
       </c>
       <c r="M3" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="N3">
         <v>500</v>
@@ -3019,7 +3016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>13</v>
       </c>
@@ -3054,10 +3051,10 @@
         <v>4505658849</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>760</v>
+        <v>784</v>
       </c>
       <c r="M4" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="N4">
         <v>75</v>
@@ -3084,7 +3081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>14</v>
       </c>
@@ -3107,7 +3104,7 @@
         <v>273</v>
       </c>
       <c r="H5" t="s">
-        <v>789</v>
+        <v>781</v>
       </c>
       <c r="I5" t="s">
         <v>252</v>
@@ -3119,10 +3116,10 @@
         <v>0</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>761</v>
+        <v>785</v>
       </c>
       <c r="M5" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="N5">
         <v>100</v>
@@ -3149,7 +3146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>15</v>
       </c>
@@ -3184,10 +3181,10 @@
         <v>5149938373</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>762</v>
+        <v>786</v>
       </c>
       <c r="M6" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="N6">
         <v>30</v>
@@ -3214,7 +3211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>16</v>
       </c>
@@ -3249,10 +3246,10 @@
         <v>0</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>763</v>
+        <v>787</v>
       </c>
       <c r="M7" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="N7">
         <v>40</v>
@@ -3279,7 +3276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>17</v>
       </c>
@@ -3314,10 +3311,10 @@
         <v>0</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>764</v>
+        <v>788</v>
       </c>
       <c r="M8" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="N8">
         <v>50</v>
@@ -3357,14 +3354,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -3375,7 +3372,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>301</v>
       </c>
@@ -3386,7 +3383,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>302</v>
       </c>
@@ -3397,7 +3394,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>303</v>
       </c>
@@ -3408,7 +3405,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>304</v>
       </c>
@@ -3431,13 +3428,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>66</v>
       </c>
@@ -3445,7 +3442,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>401</v>
       </c>
@@ -3453,7 +3450,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>402</v>
       </c>
@@ -3461,7 +3458,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>403</v>
       </c>
@@ -3481,14 +3478,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>66</v>
       </c>
@@ -3499,7 +3496,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>401</v>
       </c>
@@ -3510,7 +3507,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>401</v>
       </c>
@@ -3518,10 +3515,10 @@
         <v>302</v>
       </c>
       <c r="C3" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>401</v>
       </c>
@@ -3532,7 +3529,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>401</v>
       </c>
@@ -3543,7 +3540,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>402</v>
       </c>
@@ -3554,7 +3551,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>402</v>
       </c>
@@ -3562,10 +3559,10 @@
         <v>302</v>
       </c>
       <c r="C7" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>402</v>
       </c>
@@ -3576,7 +3573,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>402</v>
       </c>
@@ -3587,7 +3584,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>403</v>
       </c>
@@ -3595,10 +3592,10 @@
         <v>301</v>
       </c>
       <c r="C10" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>403</v>
       </c>
@@ -3609,7 +3606,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>403</v>
       </c>
@@ -3620,7 +3617,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>403</v>
       </c>
@@ -3643,14 +3640,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -3661,7 +3658,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>101</v>
       </c>
@@ -3672,7 +3669,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>102</v>
       </c>
@@ -3683,7 +3680,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>103</v>
       </c>
@@ -3694,7 +3691,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>104</v>
       </c>
@@ -3717,14 +3714,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -3735,7 +3732,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>201</v>
       </c>
@@ -3746,7 +3743,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>202</v>
       </c>
@@ -3757,7 +3754,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>203</v>
       </c>
@@ -3780,14 +3777,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>102</v>
       </c>
@@ -3798,7 +3795,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3806,7 +3803,7 @@
         <v>720</v>
       </c>
       <c r="C2" t="s">
-        <v>721</v>
+        <v>757</v>
       </c>
     </row>
   </sheetData>
@@ -3821,26 +3818,26 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -3893,15 +3890,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10001</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>768</v>
+        <v>760</v>
       </c>
       <c r="C2" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="D2" t="s">
         <v>292</v>
@@ -3919,7 +3916,7 @@
         <v>250</v>
       </c>
       <c r="I2" t="s">
-        <v>788</v>
+        <v>780</v>
       </c>
       <c r="J2" t="s">
         <v>252</v>
@@ -3946,15 +3943,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10002</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>769</v>
+        <v>761</v>
       </c>
       <c r="C3" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="D3" t="s">
         <v>296</v>
@@ -3999,15 +3996,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10003</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>770</v>
+        <v>762</v>
       </c>
       <c r="C4" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -4052,15 +4049,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10004</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>771</v>
+        <v>763</v>
       </c>
       <c r="C5" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="D5" t="s">
         <v>275</v>
@@ -4105,15 +4102,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10005</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>772</v>
+        <v>764</v>
       </c>
       <c r="C6" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -4158,15 +4155,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10006</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>773</v>
+        <v>765</v>
       </c>
       <c r="C7" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -4211,15 +4208,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10007</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>774</v>
+        <v>766</v>
       </c>
       <c r="C8" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>
@@ -4264,15 +4261,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10008</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>775</v>
+        <v>767</v>
       </c>
       <c r="C9" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="D9" t="s">
         <v>304</v>
@@ -4317,15 +4314,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10009</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>776</v>
+        <v>768</v>
       </c>
       <c r="C10" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="D10" t="s">
         <v>0</v>
@@ -4370,15 +4367,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10010</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>777</v>
+        <v>769</v>
       </c>
       <c r="C11" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
@@ -4423,15 +4420,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10011</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>778</v>
+        <v>770</v>
       </c>
       <c r="C12" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="D12" t="s">
         <v>0</v>
@@ -4476,15 +4473,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10012</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>779</v>
+        <v>771</v>
       </c>
       <c r="C13" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="D13" t="s">
         <v>0</v>
@@ -4529,15 +4526,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10013</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>780</v>
+        <v>772</v>
       </c>
       <c r="C14" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="D14" t="s">
         <v>0</v>
@@ -4582,15 +4579,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10014</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>781</v>
+        <v>773</v>
       </c>
       <c r="C15" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="D15" t="s">
         <v>307</v>
@@ -4635,15 +4632,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10015</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>782</v>
+        <v>774</v>
       </c>
       <c r="C16" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="D16" t="s">
         <v>0</v>
@@ -4688,15 +4685,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10016</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="C17" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="D17" t="s">
         <v>0</v>
@@ -4741,15 +4738,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10017</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="C18" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="D18" t="s">
         <v>0</v>
@@ -4794,15 +4791,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10018</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>785</v>
+        <v>777</v>
       </c>
       <c r="C19" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="D19" t="s">
         <v>310</v>
@@ -4847,15 +4844,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>10019</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>786</v>
+        <v>778</v>
       </c>
       <c r="C20" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="D20" t="s">
         <v>315</v>
@@ -4900,15 +4897,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>10020</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>787</v>
+        <v>779</v>
       </c>
       <c r="C21" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="D21" t="s">
         <v>320</v>
@@ -4965,14 +4962,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -4983,7 +4980,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>501</v>
       </c>
@@ -4994,7 +4991,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>502</v>
       </c>
@@ -5005,7 +5002,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>503</v>
       </c>
@@ -5016,7 +5013,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>504</v>
       </c>
@@ -5027,7 +5024,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>505</v>
       </c>
@@ -5038,7 +5035,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>506</v>
       </c>
@@ -5049,7 +5046,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>507</v>
       </c>
@@ -5060,7 +5057,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>508</v>
       </c>
@@ -5083,26 +5080,26 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="255.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="255.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="13" style="2" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.88671875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="15.44140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="8.6640625" style="2"/>
+    <col min="8" max="8" width="13.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.85546875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="15.42578125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -5146,7 +5143,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1100001</v>
       </c>
@@ -5190,7 +5187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1100002</v>
       </c>
@@ -5234,7 +5231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1100003</v>
       </c>
@@ -5278,7 +5275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1100004</v>
       </c>
@@ -5322,7 +5319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1100005</v>
       </c>
@@ -5366,7 +5363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1100006</v>
       </c>
@@ -5410,7 +5407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1100007</v>
       </c>
@@ -5454,7 +5451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1100008</v>
       </c>
@@ -5498,7 +5495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>1100009</v>
       </c>
@@ -5542,7 +5539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>1100010</v>
       </c>
@@ -5586,7 +5583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>1100011</v>
       </c>
@@ -5630,7 +5627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>1100012</v>
       </c>
@@ -5674,7 +5671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1100013</v>
       </c>
@@ -5685,7 +5682,7 @@
         <v>505</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>766</v>
+        <v>758</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>477</v>
@@ -5718,7 +5715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>1100014</v>
       </c>
@@ -5762,7 +5759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>1100015</v>
       </c>
@@ -5806,7 +5803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>1100016</v>
       </c>
@@ -5850,7 +5847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>1100017</v>
       </c>
@@ -5894,7 +5891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>1100018</v>
       </c>
@@ -5938,7 +5935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>1100019</v>
       </c>
@@ -5982,7 +5979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>1100020</v>
       </c>
@@ -6026,7 +6023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>1100021</v>
       </c>
@@ -6070,7 +6067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>1100022</v>
       </c>
@@ -6114,7 +6111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>1100023</v>
       </c>
@@ -6125,7 +6122,7 @@
         <v>506</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>767</v>
+        <v>759</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>545</v>
@@ -6158,7 +6155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>1100024</v>
       </c>
@@ -6202,7 +6199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>1100025</v>
       </c>
@@ -6246,7 +6243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>1100026</v>
       </c>
@@ -6290,7 +6287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>1100027</v>
       </c>
@@ -6334,7 +6331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>1100028</v>
       </c>
@@ -6378,7 +6375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>1100029</v>
       </c>
@@ -6422,7 +6419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>1100030</v>
       </c>
@@ -6466,7 +6463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>1100031</v>
       </c>
@@ -6510,7 +6507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>1100032</v>
       </c>
@@ -6554,7 +6551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>1200001</v>
       </c>
@@ -6598,7 +6595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>1200002</v>
       </c>
@@ -6642,7 +6639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>1200003</v>
       </c>
@@ -6686,7 +6683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>1200004</v>
       </c>
@@ -6730,7 +6727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>1200005</v>
       </c>
@@ -6774,7 +6771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>1200006</v>
       </c>
@@ -6818,7 +6815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>1200007</v>
       </c>
@@ -6862,7 +6859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>1200008</v>
       </c>
@@ -6906,7 +6903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>1200009</v>
       </c>
@@ -6950,7 +6947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>1200010</v>
       </c>
@@ -6994,7 +6991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>1200011</v>
       </c>
@@ -7038,7 +7035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>1200012</v>
       </c>
@@ -7082,7 +7079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>1200013</v>
       </c>
@@ -7126,7 +7123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>1400001</v>
       </c>
@@ -7170,7 +7167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>1400002</v>
       </c>
@@ -7214,7 +7211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>1400003</v>
       </c>
@@ -7258,7 +7255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>1400004</v>
       </c>
@@ -7302,7 +7299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>1400005</v>
       </c>
@@ -7346,7 +7343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>1400006</v>
       </c>
@@ -7390,7 +7387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>1400007</v>
       </c>
@@ -7434,7 +7431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>1400008</v>
       </c>
@@ -7478,7 +7475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>1400009</v>
       </c>
@@ -7522,7 +7519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>1400010</v>
       </c>
@@ -7566,7 +7563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>1400011</v>
       </c>
@@ -7610,7 +7607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>1400012</v>
       </c>
@@ -7654,7 +7651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>1400013</v>
       </c>
@@ -7698,7 +7695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>1400014</v>
       </c>
@@ -7742,7 +7739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>1400015</v>
       </c>
@@ -7786,7 +7783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>1400016</v>
       </c>
@@ -7830,7 +7827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>1400017</v>
       </c>
@@ -7874,7 +7871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>1400018</v>
       </c>
@@ -7918,7 +7915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>1400019</v>
       </c>
@@ -7962,7 +7959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>1600001</v>
       </c>
@@ -8006,7 +8003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>1600002</v>
       </c>
@@ -8050,7 +8047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>1600003</v>
       </c>
@@ -8094,7 +8091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>1600004</v>
       </c>
@@ -8138,7 +8135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>1600005</v>
       </c>
@@ -8182,7 +8179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>1600006</v>
       </c>
@@ -8226,7 +8223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>1600007</v>
       </c>
@@ -8270,7 +8267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>1600008</v>
       </c>
@@ -8314,7 +8311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>1600009</v>
       </c>
@@ -8358,7 +8355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>1600010</v>
       </c>
@@ -8402,7 +8399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>1600011</v>
       </c>
@@ -8446,7 +8443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>1600012</v>
       </c>
@@ -8490,7 +8487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>1600013</v>
       </c>
@@ -8534,7 +8531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>1600014</v>
       </c>
@@ -8578,7 +8575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>1600015</v>
       </c>
@@ -8622,7 +8619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>1600016</v>
       </c>
@@ -8666,7 +8663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>1600017</v>
       </c>
@@ -8710,7 +8707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>1600018</v>
       </c>
@@ -8754,7 +8751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>1600019</v>
       </c>
@@ -8798,7 +8795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>1600020</v>
       </c>
@@ -8842,7 +8839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>1600021</v>
       </c>
@@ -8886,7 +8883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>1600022</v>
       </c>
@@ -8930,7 +8927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>1600023</v>
       </c>
@@ -8974,7 +8971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>1600024</v>
       </c>
@@ -9018,7 +9015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>1600025</v>
       </c>
@@ -9062,7 +9059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>1600026</v>
       </c>
@@ -9106,7 +9103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>1600027</v>
       </c>
@@ -9150,7 +9147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>1600028</v>
       </c>
@@ -9194,7 +9191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>1600029</v>
       </c>
@@ -9238,7 +9235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>1600030</v>
       </c>
@@ -9282,7 +9279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>1600031</v>
       </c>
@@ -9326,7 +9323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>1600032</v>
       </c>
@@ -9370,7 +9367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>1600033</v>
       </c>
@@ -9414,7 +9411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>1600034</v>
       </c>
@@ -9458,7 +9455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>1600035</v>
       </c>
@@ -9502,7 +9499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>1600036</v>
       </c>
@@ -9546,7 +9543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>1600037</v>
       </c>
@@ -9590,7 +9587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>1600038</v>
       </c>
@@ -9634,7 +9631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>1600039</v>
       </c>
@@ -9678,7 +9675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>1600040</v>
       </c>
@@ -9735,17 +9732,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -9765,7 +9762,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -9785,7 +9782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -9805,7 +9802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -9825,7 +9822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -9845,7 +9842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -9865,7 +9862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -9885,7 +9882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -9905,7 +9902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -9925,7 +9922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -9945,7 +9942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -9965,7 +9962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -9985,7 +9982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -10005,7 +10002,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -10025,7 +10022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -10045,7 +10042,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -10065,7 +10062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -10085,7 +10082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -10105,7 +10102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -10125,7 +10122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -10145,7 +10142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -10165,7 +10162,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -10185,7 +10182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -10205,7 +10202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -10225,7 +10222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -10245,7 +10242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -10265,7 +10262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -10285,7 +10282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -10305,7 +10302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -10325,7 +10322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -10357,23 +10354,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -10411,7 +10408,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -10449,7 +10446,7 @@
         <v>4389</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -10487,7 +10484,7 @@
         <v>1707</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -10525,7 +10522,7 @@
         <v>3107</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -10563,7 +10560,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -10583,7 +10580,7 @@
         <v>402</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="H6" t="s">
         <v>717</v>
@@ -10601,7 +10598,7 @@
         <v>3389</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -10639,7 +10636,7 @@
         <v>4472</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -10677,7 +10674,7 @@
         <v>3957</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -10715,7 +10712,7 @@
         <v>3259</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -10735,7 +10732,7 @@
         <v>401</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="H10" t="s">
         <v>693</v>
@@ -10753,7 +10750,7 @@
         <v>3283</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -10773,7 +10770,7 @@
         <v>401</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="H11" t="s">
         <v>694</v>
@@ -10791,7 +10788,7 @@
         <v>2627</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -10811,7 +10808,7 @@
         <v>402</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H12" t="s">
         <v>696</v>
@@ -10829,7 +10826,7 @@
         <v>1283</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -10867,7 +10864,7 @@
         <v>1888</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -10905,7 +10902,7 @@
         <v>4183</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -10925,7 +10922,7 @@
         <v>401</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="H15" t="s">
         <v>698</v>
@@ -10943,7 +10940,7 @@
         <v>4430</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -10981,7 +10978,7 @@
         <v>4598</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -11019,7 +11016,7 @@
         <v>3639</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -11070,16 +11067,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -11096,7 +11093,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -11113,7 +11110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -11130,7 +11127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -11147,7 +11144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -11164,7 +11161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -11181,7 +11178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -11198,7 +11195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -11215,7 +11212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -11232,7 +11229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -11249,7 +11246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -11266,7 +11263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -11283,7 +11280,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -11300,7 +11297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -11317,7 +11314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -11334,7 +11331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -11351,7 +11348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -11368,7 +11365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -11385,7 +11382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -11402,7 +11399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -11419,7 +11416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -11436,7 +11433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -11453,7 +11450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -11470,7 +11467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -11487,7 +11484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -11504,7 +11501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -11521,7 +11518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -11538,7 +11535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -11555,7 +11552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -11572,7 +11569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -11589,7 +11586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -11606,7 +11603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -11623,7 +11620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -11640,7 +11637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -11657,7 +11654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -11674,7 +11671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -11691,7 +11688,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -11708,7 +11705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -11725,7 +11722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -11742,7 +11739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -11759,7 +11756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -11776,7 +11773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -11793,7 +11790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -11822,14 +11819,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -11840,7 +11837,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11</v>
       </c>
@@ -11851,7 +11848,7 @@
         <v>43477.417071759257</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>11</v>
       </c>
@@ -11862,7 +11859,7 @@
         <v>43477.418182870373</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>11</v>
       </c>
@@ -11873,7 +11870,7 @@
         <v>43477.420694444445</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>11</v>
       </c>
@@ -11884,7 +11881,7 @@
         <v>43477.459050925929</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>11</v>
       </c>
@@ -11895,7 +11892,7 @@
         <v>43477.460497685184</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>11</v>
       </c>
@@ -11906,7 +11903,7 @@
         <v>43477.461770833332</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>11</v>
       </c>
@@ -11917,7 +11914,7 @@
         <v>43478.544317129628</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>11</v>
       </c>
@@ -11928,7 +11925,7 @@
         <v>43478.552187499998</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>11</v>
       </c>
@@ -11939,7 +11936,7 @@
         <v>43478.594386574077</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
@@ -11950,7 +11947,7 @@
         <v>43478.596458333333</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -11961,7 +11958,7 @@
         <v>43478.628842592596</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -11972,7 +11969,7 @@
         <v>43478.636087962965</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -11983,7 +11980,7 @@
         <v>43482.754201388889</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -11994,7 +11991,7 @@
         <v>43484.417743055557</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>11</v>
       </c>
@@ -12005,7 +12002,7 @@
         <v>43484.422546296293</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11</v>
       </c>
@@ -12016,7 +12013,7 @@
         <v>43484.42291666667</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>12</v>
       </c>
@@ -12027,7 +12024,7 @@
         <v>43484.426423611112</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>12</v>
       </c>
@@ -12038,7 +12035,7 @@
         <v>43484.431192129632</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>12</v>
       </c>
@@ -12049,7 +12046,7 @@
         <v>43484.43241898148</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>12</v>
       </c>
@@ -12060,7 +12057,7 @@
         <v>43484.434259259258</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>12</v>
       </c>
@@ -12071,7 +12068,7 @@
         <v>43484.460717592592</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>12</v>
       </c>
@@ -12082,7 +12079,7 @@
         <v>43484.462060185186</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>12</v>
       </c>
@@ -12093,7 +12090,7 @@
         <v>43484.462858796294</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>12</v>
       </c>
@@ -12104,7 +12101,7 @@
         <v>43484.466307870367</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>12</v>
       </c>
@@ -12115,7 +12112,7 @@
         <v>43484.470775462964</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>12</v>
       </c>
@@ -12126,7 +12123,7 @@
         <v>43484.475682870368</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>12</v>
       </c>
@@ -12137,7 +12134,7 @@
         <v>43484.481122685182</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>12</v>
       </c>
@@ -12148,7 +12145,7 @@
         <v>43484.545046296298</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>14</v>
       </c>
@@ -12159,7 +12156,7 @@
         <v>43484.547118055554</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>14</v>
       </c>
@@ -12170,7 +12167,7 @@
         <v>43484.548460648148</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>14</v>
       </c>
@@ -12181,7 +12178,7 @@
         <v>43484.551631944443</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>14</v>
       </c>
@@ -12192,7 +12189,7 @@
         <v>43484.552407407406</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>14</v>
       </c>
@@ -12203,7 +12200,7 @@
         <v>43484.557893518519</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>14</v>
       </c>
@@ -12214,7 +12211,7 @@
         <v>43484.561956018515</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>11</v>
       </c>
@@ -12225,7 +12222,7 @@
         <v>43485.547951388886</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>11</v>
       </c>
@@ -12236,7 +12233,7 @@
         <v>43485.553495370368</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>12</v>
       </c>
@@ -12247,7 +12244,7 @@
         <v>43485.5546875</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>12</v>
       </c>
@@ -12258,7 +12255,7 @@
         <v>43485.557916666665</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>12</v>
       </c>
@@ -12269,7 +12266,7 @@
         <v>43485.560243055559</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>12</v>
       </c>
@@ -12280,7 +12277,7 @@
         <v>43485.56453703704</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>12</v>
       </c>
@@ -12291,7 +12288,7 @@
         <v>43485.565057870372</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>12</v>
       </c>
@@ -12302,7 +12299,7 @@
         <v>43485.587997685187</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>12</v>
       </c>
@@ -12313,7 +12310,7 @@
         <v>43485.590127314812</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>12</v>
       </c>
@@ -12324,7 +12321,7 @@
         <v>43485.59578703704</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>12</v>
       </c>
@@ -12335,7 +12332,7 @@
         <v>43485.601377314815</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>12</v>
       </c>
@@ -12346,7 +12343,7 @@
         <v>43485.60664351852</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>12</v>
       </c>
@@ -12357,7 +12354,7 @@
         <v>43485.609884259262</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>14</v>
       </c>
@@ -12368,7 +12365,7 @@
         <v>43485.614710648151</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>14</v>
       </c>
@@ -12379,7 +12376,7 @@
         <v>43485.61791666667</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>14</v>
       </c>
@@ -12390,7 +12387,7 @@
         <v>43485.626550925925</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>14</v>
       </c>
@@ -12401,7 +12398,7 @@
         <v>43485.629050925927</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>14</v>
       </c>
@@ -12412,7 +12409,7 @@
         <v>43485.63449074074</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>14</v>
       </c>
@@ -12423,7 +12420,7 @@
         <v>43485.638425925928</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>16</v>
       </c>
@@ -12434,7 +12431,7 @@
         <v>43485.64303240741</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>16</v>
       </c>
@@ -12445,7 +12442,7 @@
         <v>43485.647696759261</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>16</v>
       </c>
@@ -12456,7 +12453,7 @@
         <v>43485.651388888888</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>16</v>
       </c>
@@ -12467,7 +12464,7 @@
         <v>43485.653807870367</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>16</v>
       </c>
@@ -12478,7 +12475,7 @@
         <v>43485.659224537034</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>16</v>
       </c>
@@ -12489,7 +12486,7 @@
         <v>43486.750844907408</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>14</v>
       </c>
@@ -12500,7 +12497,7 @@
         <v>43486.767256944448</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>11</v>
       </c>
@@ -12512,7 +12509,7 @@
       </c>
       <c r="E62" s="1"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>14</v>
       </c>
@@ -12523,7 +12520,7 @@
         <v>43488.751446759263</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>12</v>
       </c>
@@ -12534,7 +12531,7 @@
         <v>43489.75099537037</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>12</v>
       </c>
@@ -12545,7 +12542,7 @@
         <v>43490.792407407411</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>12</v>
       </c>
@@ -12556,7 +12553,7 @@
         <v>43491.416898148149</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>11</v>
       </c>
@@ -12567,7 +12564,7 @@
         <v>43491.423159722224</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>12</v>
       </c>
@@ -12578,7 +12575,7 @@
         <v>43491.428483796299</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>12</v>
       </c>
@@ -12589,7 +12586,7 @@
         <v>43491.433634259258</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>12</v>
       </c>
@@ -12600,7 +12597,7 @@
         <v>43491.443773148145</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>12</v>
       </c>
@@ -12611,7 +12608,7 @@
         <v>43491.460578703707</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>12</v>
       </c>
@@ -12622,7 +12619,7 @@
         <v>43491.466435185182</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>12</v>
       </c>
@@ -12633,7 +12630,7 @@
         <v>43491.466863425929</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>12</v>
       </c>
@@ -12644,7 +12641,7 @@
         <v>43491.469293981485</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>12</v>
       </c>
@@ -12655,7 +12652,7 @@
         <v>43491.471574074072</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>14</v>
       </c>
@@ -12666,7 +12663,7 @@
         <v>43491.472384259258</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>14</v>
       </c>
@@ -12677,7 +12674,7 @@
         <v>43491.547118055554</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>14</v>
       </c>
@@ -12688,7 +12685,7 @@
         <v>43491.548460648148</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>14</v>
       </c>
@@ -12699,7 +12696,7 @@
         <v>43491.553715277776</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>14</v>
       </c>
@@ -12710,7 +12707,7 @@
         <v>43491.558009259257</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>16</v>
       </c>
@@ -12721,7 +12718,7 @@
         <v>43491.562002314815</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>16</v>
       </c>
@@ -12732,7 +12729,7 @@
         <v>43491.565486111111</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>16</v>
       </c>
@@ -12743,7 +12740,7 @@
         <v>43491.56690972222</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>16</v>
       </c>
@@ -12754,7 +12751,7 @@
         <v>43491.569699074076</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>11</v>
       </c>
@@ -12765,7 +12762,7 @@
         <v>43492.546018518522</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>12</v>
       </c>
@@ -12776,7 +12773,7 @@
         <v>43492.549930555557</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>12</v>
       </c>
@@ -12787,7 +12784,7 @@
         <v>43492.552430555559</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>12</v>
       </c>
@@ -12798,7 +12795,7 @@
         <v>43492.555543981478</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>12</v>
       </c>
@@ -12809,7 +12806,7 @@
         <v>43492.556539351855</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>12</v>
       </c>
@@ -12820,7 +12817,7 @@
         <v>43492.586678240739</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>12</v>
       </c>
@@ -12831,7 +12828,7 @@
         <v>43492.587060185186</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>12</v>
       </c>
@@ -12842,7 +12839,7 @@
         <v>43492.591527777775</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>12</v>
       </c>
@@ -12853,7 +12850,7 @@
         <v>43492.595983796295</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>14</v>
       </c>
@@ -12864,7 +12861,7 @@
         <v>43492.597268518519</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>14</v>
       </c>
@@ -12875,7 +12872,7 @@
         <v>43492.630497685182</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>16</v>
       </c>
@@ -12886,7 +12883,7 @@
         <v>43492.634293981479</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>16</v>
       </c>
@@ -12897,7 +12894,7 @@
         <v>43492.636354166665</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>16</v>
       </c>
@@ -12908,7 +12905,7 @@
         <v>43492.643391203703</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>16</v>
       </c>
@@ -12919,7 +12916,7 @@
         <v>43492.644317129627</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>16</v>
       </c>
@@ -12930,7 +12927,7 @@
         <v>43493.731493055559</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>16</v>
       </c>
@@ -12941,7 +12938,7 @@
         <v>43493.735914351855</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>16</v>
       </c>
@@ -12952,7 +12949,7 @@
         <v>43493.739560185182</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>14</v>
       </c>
@@ -12963,7 +12960,7 @@
         <v>43495.751099537039</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>12</v>
       </c>
@@ -12974,7 +12971,7 @@
         <v>43495.761493055557</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>12</v>
       </c>
@@ -12985,7 +12982,7 @@
         <v>43496.751493055555</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>12</v>
       </c>
@@ -12996,7 +12993,7 @@
         <v>43497.796087962961</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>12</v>
       </c>
@@ -13007,7 +13004,7 @@
         <v>43497.797615740739</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>11</v>
       </c>
@@ -13018,7 +13015,7 @@
         <v>43498.418240740742</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>12</v>
       </c>
@@ -13029,7 +13026,7 @@
         <v>43498.423067129632</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>11</v>
       </c>
@@ -13040,7 +13037,7 @@
         <v>43498.427372685182</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>12</v>
       </c>
@@ -13051,7 +13048,7 @@
         <v>43498.462719907409</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>12</v>
       </c>
@@ -13062,7 +13059,7 @@
         <v>43498.465057870373</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>12</v>
       </c>
@@ -13073,7 +13070,7 @@
         <v>43498.467199074075</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>12</v>
       </c>
@@ -13084,7 +13081,7 @@
         <v>43498.545405092591</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>14</v>
       </c>
@@ -13095,7 +13092,7 @@
         <v>43498.550034722219</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>14</v>
       </c>
@@ -13106,7 +13103,7 @@
         <v>43498.550763888888</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>16</v>
       </c>
@@ -13117,7 +13114,7 @@
         <v>43498.556620370371</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>16</v>
       </c>
@@ -13128,7 +13125,7 @@
         <v>43498.557615740741</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>14</v>
       </c>
@@ -13139,7 +13136,7 @@
         <v>43499.543877314813</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>12</v>
       </c>
@@ -13150,7 +13147,7 @@
         <v>43499.544965277775</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>12</v>
       </c>
@@ -13161,7 +13158,7 @@
         <v>43499.546701388892</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>12</v>
       </c>
@@ -13172,7 +13169,7 @@
         <v>43499.586701388886</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>12</v>
       </c>
@@ -13183,7 +13180,7 @@
         <v>43499.587500000001</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>14</v>
       </c>
@@ -13194,7 +13191,7 @@
         <v>43499.590636574074</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>14</v>
       </c>
@@ -13205,7 +13202,7 @@
         <v>43499.632280092592</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>16</v>
       </c>
@@ -13216,7 +13213,7 @@
         <v>43499.635312500002</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>16</v>
       </c>
@@ -13240,23 +13237,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -13294,7 +13291,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -13317,7 +13314,7 @@
         <v>4389</v>
       </c>
       <c r="H2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="I2" t="s">
         <v>253</v>
@@ -13332,7 +13329,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -13355,10 +13352,10 @@
         <v>1707</v>
       </c>
       <c r="H3" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="I3" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="J3" t="s">
         <v>683</v>
@@ -13370,7 +13367,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -13393,7 +13390,7 @@
         <v>3107</v>
       </c>
       <c r="H4" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="I4" t="s">
         <v>687</v>
@@ -13408,7 +13405,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -13431,10 +13428,10 @@
         <v>1042</v>
       </c>
       <c r="H5" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="I5" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="J5" t="s">
         <v>683</v>
@@ -13446,12 +13443,12 @@
         <v>705</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="C6">
         <v>16</v>
@@ -13469,10 +13466,10 @@
         <v>3389</v>
       </c>
       <c r="H6" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="I6" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="J6" t="s">
         <v>551</v>
@@ -13484,7 +13481,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -13507,10 +13504,10 @@
         <v>4472</v>
       </c>
       <c r="H7" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="I7" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="J7" t="s">
         <v>683</v>
@@ -13522,7 +13519,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -13545,7 +13542,7 @@
         <v>3957</v>
       </c>
       <c r="H8" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="I8" t="s">
         <v>691</v>
@@ -13560,7 +13557,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -13583,7 +13580,7 @@
         <v>3259</v>
       </c>
       <c r="H9" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="I9" t="s">
         <v>692</v>
@@ -13598,12 +13595,12 @@
         <v>708</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C10">
         <v>12</v>
@@ -13621,10 +13618,10 @@
         <v>3283</v>
       </c>
       <c r="H10" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="I10" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="J10" t="s">
         <v>684</v>
@@ -13636,12 +13633,12 @@
         <v>709</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C11">
         <v>16</v>
@@ -13659,10 +13656,10 @@
         <v>2627</v>
       </c>
       <c r="H11" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="I11" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="J11" t="s">
         <v>684</v>
@@ -13674,12 +13671,12 @@
         <v>710</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C12">
         <v>14</v>
@@ -13697,10 +13694,10 @@
         <v>1283</v>
       </c>
       <c r="H12" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="I12" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="J12" t="s">
         <v>685</v>
@@ -13712,7 +13709,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -13735,7 +13732,7 @@
         <v>1888</v>
       </c>
       <c r="H13" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="I13" t="s">
         <v>695</v>
@@ -13750,7 +13747,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -13773,10 +13770,10 @@
         <v>4183</v>
       </c>
       <c r="H14" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="I14" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="J14" t="s">
         <v>683</v>
@@ -13788,12 +13785,12 @@
         <v>683</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C15">
         <v>12</v>
@@ -13811,10 +13808,10 @@
         <v>4430</v>
       </c>
       <c r="H15" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="I15" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="J15" t="s">
         <v>686</v>
@@ -13826,7 +13823,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -13849,10 +13846,10 @@
         <v>4598</v>
       </c>
       <c r="H16" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="I16" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="J16" t="s">
         <v>683</v>
@@ -13864,7 +13861,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -13887,10 +13884,10 @@
         <v>3639</v>
       </c>
       <c r="H17" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="I17" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="J17" t="s">
         <v>551</v>
@@ -13902,7 +13899,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -13925,7 +13922,7 @@
         <v>2937</v>
       </c>
       <c r="H18" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="I18" t="s">
         <v>701</v>

</xml_diff>

<commit_message>
Update courriels vendeur et gestionnaire, vendeur...@gmail.com et gestionnaire1@gmail.com
</commit_message>
<xml_diff>
--- a/Jeu d'essai.xlsx
+++ b/Jeu d'essai.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="134" documentId="114_{8D9B191C-2013-4270-87A9-3FB899E57325}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{4DE29F17-CD87-41D4-A643-08A4CC30A177}"/>
+  <xr:revisionPtr revIDLastSave="145" documentId="114_{8D9B191C-2013-4270-87A9-3FB899E57325}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{C7C63C9A-166B-40C8-9094-0DB7A69481D7}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PPVendeurs" sheetId="13" r:id="rId1"/>
@@ -2256,9 +2256,6 @@
     <t>1100013.JPG</t>
   </si>
   <si>
-    <t>ppuces@gmail.com</t>
-  </si>
-  <si>
     <t>203.99</t>
   </si>
   <si>
@@ -2442,25 +2439,28 @@
     <t>K0H1Y0</t>
   </si>
   <si>
-    <t>vendeur11@outlook.com</t>
-  </si>
-  <si>
-    <t>vendeur12@outlook.com</t>
-  </si>
-  <si>
-    <t>vendeur13@outlook.com</t>
-  </si>
-  <si>
-    <t>vendeur14@outlook.com</t>
-  </si>
-  <si>
-    <t>vendeur15@outlook.com</t>
-  </si>
-  <si>
-    <t>vendeur16@outlook.com</t>
-  </si>
-  <si>
-    <t>vendeur17@outlook.com</t>
+    <t>vendeur11@gmail.com</t>
+  </si>
+  <si>
+    <t>vendeur12@gmail.com</t>
+  </si>
+  <si>
+    <t>vendeur13@gmail.com</t>
+  </si>
+  <si>
+    <t>vendeur14@gmail.com</t>
+  </si>
+  <si>
+    <t>vendeur15@gmail.com</t>
+  </si>
+  <si>
+    <t>vendeur16@gmail.com</t>
+  </si>
+  <si>
+    <t>vendeur17@gmail.com</t>
+  </si>
+  <si>
+    <t>gestionnaire1@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2798,30 +2798,30 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>11</v>
       </c>
@@ -2921,10 +2921,10 @@
         <v>0</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="M2" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="N2">
         <v>500</v>
@@ -2951,7 +2951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>12</v>
       </c>
@@ -2986,10 +2986,10 @@
         <v>0</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="M3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="N3">
         <v>500</v>
@@ -3016,7 +3016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>13</v>
       </c>
@@ -3051,10 +3051,10 @@
         <v>4505658849</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="M4" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="N4">
         <v>75</v>
@@ -3081,7 +3081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>14</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>273</v>
       </c>
       <c r="H5" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="I5" t="s">
         <v>252</v>
@@ -3116,10 +3116,10 @@
         <v>0</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="M5" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="N5">
         <v>100</v>
@@ -3146,7 +3146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>15</v>
       </c>
@@ -3181,10 +3181,10 @@
         <v>5149938373</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="M6" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="N6">
         <v>30</v>
@@ -3211,7 +3211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>16</v>
       </c>
@@ -3246,10 +3246,10 @@
         <v>0</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="M7" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="N7">
         <v>40</v>
@@ -3276,7 +3276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>17</v>
       </c>
@@ -3311,10 +3311,10 @@
         <v>0</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="M8" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="N8">
         <v>50</v>
@@ -3354,14 +3354,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>301</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>302</v>
       </c>
@@ -3394,7 +3394,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>303</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>304</v>
       </c>
@@ -3428,13 +3428,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>66</v>
       </c>
@@ -3442,7 +3442,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>401</v>
       </c>
@@ -3450,7 +3450,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>402</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>403</v>
       </c>
@@ -3478,14 +3478,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>66</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>401</v>
       </c>
@@ -3507,7 +3507,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>401</v>
       </c>
@@ -3515,10 +3515,10 @@
         <v>302</v>
       </c>
       <c r="C3" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>401</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>401</v>
       </c>
@@ -3540,7 +3540,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>402</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>402</v>
       </c>
@@ -3559,10 +3559,10 @@
         <v>302</v>
       </c>
       <c r="C7" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>402</v>
       </c>
@@ -3573,7 +3573,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>402</v>
       </c>
@@ -3584,7 +3584,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>403</v>
       </c>
@@ -3592,10 +3592,10 @@
         <v>301</v>
       </c>
       <c r="C10" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>403</v>
       </c>
@@ -3606,7 +3606,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>403</v>
       </c>
@@ -3617,7 +3617,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>403</v>
       </c>
@@ -3640,14 +3640,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -3658,7 +3658,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>101</v>
       </c>
@@ -3669,7 +3669,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>102</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>103</v>
       </c>
@@ -3691,7 +3691,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>104</v>
       </c>
@@ -3714,14 +3714,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -3732,7 +3732,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>201</v>
       </c>
@@ -3743,7 +3743,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>202</v>
       </c>
@@ -3754,7 +3754,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>203</v>
       </c>
@@ -3777,14 +3777,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>102</v>
       </c>
@@ -3795,15 +3795,15 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>720</v>
+        <v>788</v>
       </c>
       <c r="C2" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
   </sheetData>
@@ -3818,26 +3818,26 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -3890,15 +3890,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10001</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C2" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D2" t="s">
         <v>292</v>
@@ -3916,7 +3916,7 @@
         <v>250</v>
       </c>
       <c r="I2" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="J2" t="s">
         <v>252</v>
@@ -3943,15 +3943,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10002</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D3" t="s">
         <v>296</v>
@@ -3996,15 +3996,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10003</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C4" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -4049,15 +4049,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10004</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C5" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D5" t="s">
         <v>275</v>
@@ -4102,15 +4102,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10005</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C6" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -4155,15 +4155,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10006</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C7" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -4208,15 +4208,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10007</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C8" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>
@@ -4261,15 +4261,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10008</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C9" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D9" t="s">
         <v>304</v>
@@ -4314,15 +4314,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10009</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C10" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D10" t="s">
         <v>0</v>
@@ -4367,15 +4367,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10010</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C11" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
@@ -4420,15 +4420,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10011</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="C12" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D12" t="s">
         <v>0</v>
@@ -4473,15 +4473,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10012</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="C13" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D13" t="s">
         <v>0</v>
@@ -4526,15 +4526,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>10013</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="C14" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D14" t="s">
         <v>0</v>
@@ -4579,15 +4579,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10014</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C15" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D15" t="s">
         <v>307</v>
@@ -4632,15 +4632,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10015</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="C16" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D16" t="s">
         <v>0</v>
@@ -4685,15 +4685,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>10016</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C17" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D17" t="s">
         <v>0</v>
@@ -4738,15 +4738,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>10017</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="C18" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D18" t="s">
         <v>0</v>
@@ -4791,15 +4791,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>10018</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C19" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D19" t="s">
         <v>310</v>
@@ -4844,15 +4844,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>10019</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="C20" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D20" t="s">
         <v>315</v>
@@ -4897,15 +4897,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>10020</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C21" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D21" t="s">
         <v>320</v>
@@ -4962,14 +4962,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -4980,7 +4980,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>501</v>
       </c>
@@ -4991,7 +4991,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>502</v>
       </c>
@@ -5002,7 +5002,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>503</v>
       </c>
@@ -5013,7 +5013,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>504</v>
       </c>
@@ -5024,7 +5024,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>505</v>
       </c>
@@ -5035,7 +5035,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>506</v>
       </c>
@@ -5046,7 +5046,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>507</v>
       </c>
@@ -5057,7 +5057,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>508</v>
       </c>
@@ -5080,26 +5080,26 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="255.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="255.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="13" style="2" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.85546875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="8.7109375" style="2"/>
+    <col min="8" max="8" width="13.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.88671875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="15.44140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -5143,7 +5143,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1100001</v>
       </c>
@@ -5187,7 +5187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1100002</v>
       </c>
@@ -5231,7 +5231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1100003</v>
       </c>
@@ -5275,7 +5275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>1100004</v>
       </c>
@@ -5319,7 +5319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>1100005</v>
       </c>
@@ -5363,7 +5363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>1100006</v>
       </c>
@@ -5407,7 +5407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>1100007</v>
       </c>
@@ -5451,7 +5451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>1100008</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>1100009</v>
       </c>
@@ -5539,7 +5539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>1100010</v>
       </c>
@@ -5583,7 +5583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>1100011</v>
       </c>
@@ -5627,7 +5627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>1100012</v>
       </c>
@@ -5671,7 +5671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>1100013</v>
       </c>
@@ -5682,7 +5682,7 @@
         <v>505</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>477</v>
@@ -5715,7 +5715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>1100014</v>
       </c>
@@ -5759,7 +5759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>1100015</v>
       </c>
@@ -5803,7 +5803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>1100016</v>
       </c>
@@ -5847,7 +5847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>1100017</v>
       </c>
@@ -5891,7 +5891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>1100018</v>
       </c>
@@ -5935,7 +5935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>1100019</v>
       </c>
@@ -5979,7 +5979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>1100020</v>
       </c>
@@ -6023,7 +6023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>1100021</v>
       </c>
@@ -6067,7 +6067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>1100022</v>
       </c>
@@ -6111,7 +6111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>1100023</v>
       </c>
@@ -6122,7 +6122,7 @@
         <v>506</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>545</v>
@@ -6155,7 +6155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>1100024</v>
       </c>
@@ -6199,7 +6199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>1100025</v>
       </c>
@@ -6243,7 +6243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>1100026</v>
       </c>
@@ -6287,7 +6287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>1100027</v>
       </c>
@@ -6331,7 +6331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>1100028</v>
       </c>
@@ -6375,7 +6375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>1100029</v>
       </c>
@@ -6419,7 +6419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>1100030</v>
       </c>
@@ -6463,7 +6463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>1100031</v>
       </c>
@@ -6507,7 +6507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>1100032</v>
       </c>
@@ -6551,7 +6551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>1200001</v>
       </c>
@@ -6595,7 +6595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>1200002</v>
       </c>
@@ -6639,7 +6639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>1200003</v>
       </c>
@@ -6683,7 +6683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>1200004</v>
       </c>
@@ -6727,7 +6727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>1200005</v>
       </c>
@@ -6771,7 +6771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>1200006</v>
       </c>
@@ -6815,7 +6815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>1200007</v>
       </c>
@@ -6859,7 +6859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>1200008</v>
       </c>
@@ -6903,7 +6903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>1200009</v>
       </c>
@@ -6947,7 +6947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>1200010</v>
       </c>
@@ -6991,7 +6991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>1200011</v>
       </c>
@@ -7035,7 +7035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>1200012</v>
       </c>
@@ -7079,7 +7079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>1200013</v>
       </c>
@@ -7123,7 +7123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>1400001</v>
       </c>
@@ -7167,7 +7167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>1400002</v>
       </c>
@@ -7211,7 +7211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>1400003</v>
       </c>
@@ -7255,7 +7255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>1400004</v>
       </c>
@@ -7299,7 +7299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>1400005</v>
       </c>
@@ -7343,7 +7343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>1400006</v>
       </c>
@@ -7387,7 +7387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>1400007</v>
       </c>
@@ -7431,7 +7431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>1400008</v>
       </c>
@@ -7475,7 +7475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>1400009</v>
       </c>
@@ -7519,7 +7519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>1400010</v>
       </c>
@@ -7563,7 +7563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>1400011</v>
       </c>
@@ -7607,7 +7607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>1400012</v>
       </c>
@@ -7651,7 +7651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>1400013</v>
       </c>
@@ -7695,7 +7695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>1400014</v>
       </c>
@@ -7739,7 +7739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>1400015</v>
       </c>
@@ -7783,7 +7783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>1400016</v>
       </c>
@@ -7827,7 +7827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>1400017</v>
       </c>
@@ -7871,7 +7871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>1400018</v>
       </c>
@@ -7915,7 +7915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>1400019</v>
       </c>
@@ -7959,7 +7959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>1600001</v>
       </c>
@@ -8003,7 +8003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>1600002</v>
       </c>
@@ -8047,7 +8047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>1600003</v>
       </c>
@@ -8091,7 +8091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>1600004</v>
       </c>
@@ -8135,7 +8135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>1600005</v>
       </c>
@@ -8179,7 +8179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>1600006</v>
       </c>
@@ -8223,7 +8223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>1600007</v>
       </c>
@@ -8267,7 +8267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>1600008</v>
       </c>
@@ -8311,7 +8311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>1600009</v>
       </c>
@@ -8355,7 +8355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>1600010</v>
       </c>
@@ -8399,7 +8399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>1600011</v>
       </c>
@@ -8443,7 +8443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>1600012</v>
       </c>
@@ -8487,7 +8487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>1600013</v>
       </c>
@@ -8531,7 +8531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>1600014</v>
       </c>
@@ -8575,7 +8575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>1600015</v>
       </c>
@@ -8619,7 +8619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>1600016</v>
       </c>
@@ -8663,7 +8663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>1600017</v>
       </c>
@@ -8707,7 +8707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>1600018</v>
       </c>
@@ -8751,7 +8751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>1600019</v>
       </c>
@@ -8795,7 +8795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>1600020</v>
       </c>
@@ -8839,7 +8839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>1600021</v>
       </c>
@@ -8883,7 +8883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>1600022</v>
       </c>
@@ -8927,7 +8927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>1600023</v>
       </c>
@@ -8971,7 +8971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>1600024</v>
       </c>
@@ -9015,7 +9015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>1600025</v>
       </c>
@@ -9059,7 +9059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>1600026</v>
       </c>
@@ -9103,7 +9103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <v>1600027</v>
       </c>
@@ -9147,7 +9147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <v>1600028</v>
       </c>
@@ -9191,7 +9191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <v>1600029</v>
       </c>
@@ -9235,7 +9235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
         <v>1600030</v>
       </c>
@@ -9279,7 +9279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>1600031</v>
       </c>
@@ -9323,7 +9323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>1600032</v>
       </c>
@@ -9367,7 +9367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>1600033</v>
       </c>
@@ -9411,7 +9411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <v>1600034</v>
       </c>
@@ -9455,7 +9455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <v>1600035</v>
       </c>
@@ -9499,7 +9499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <v>1600036</v>
       </c>
@@ -9543,7 +9543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <v>1600037</v>
       </c>
@@ -9587,7 +9587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>1600038</v>
       </c>
@@ -9631,7 +9631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
         <v>1600039</v>
       </c>
@@ -9675,7 +9675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
         <v>1600040</v>
       </c>
@@ -9732,17 +9732,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -9762,7 +9762,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -9782,7 +9782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -9802,7 +9802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -9822,7 +9822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -9842,7 +9842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -9862,7 +9862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -9882,7 +9882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -9902,7 +9902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -9922,7 +9922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -9942,7 +9942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -9962,7 +9962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -9982,7 +9982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -10002,7 +10002,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -10022,7 +10022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -10042,7 +10042,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -10062,7 +10062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -10082,7 +10082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -10102,7 +10102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -10122,7 +10122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -10142,7 +10142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -10162,7 +10162,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -10182,7 +10182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -10202,7 +10202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -10222,7 +10222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -10242,7 +10242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -10262,7 +10262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -10282,7 +10282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -10302,7 +10302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -10322,7 +10322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -10354,23 +10354,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -10408,7 +10408,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -10446,7 +10446,7 @@
         <v>4389</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -10484,7 +10484,7 @@
         <v>1707</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -10522,7 +10522,7 @@
         <v>3107</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -10560,7 +10560,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -10580,7 +10580,7 @@
         <v>402</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="H6" t="s">
         <v>717</v>
@@ -10598,7 +10598,7 @@
         <v>3389</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -10636,7 +10636,7 @@
         <v>4472</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -10674,7 +10674,7 @@
         <v>3957</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -10712,7 +10712,7 @@
         <v>3259</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -10732,7 +10732,7 @@
         <v>401</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="H10" t="s">
         <v>693</v>
@@ -10750,7 +10750,7 @@
         <v>3283</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -10770,7 +10770,7 @@
         <v>401</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="H11" t="s">
         <v>694</v>
@@ -10788,7 +10788,7 @@
         <v>2627</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -10808,7 +10808,7 @@
         <v>402</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="H12" t="s">
         <v>696</v>
@@ -10826,7 +10826,7 @@
         <v>1283</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -10864,7 +10864,7 @@
         <v>1888</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -10902,7 +10902,7 @@
         <v>4183</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -10922,7 +10922,7 @@
         <v>401</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H15" t="s">
         <v>698</v>
@@ -10940,7 +10940,7 @@
         <v>4430</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -10978,7 +10978,7 @@
         <v>4598</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -11016,7 +11016,7 @@
         <v>3639</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -11067,16 +11067,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -11093,7 +11093,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -11110,7 +11110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -11127,7 +11127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -11144,7 +11144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -11161,7 +11161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -11178,7 +11178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -11195,7 +11195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -11212,7 +11212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -11229,7 +11229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -11246,7 +11246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -11263,7 +11263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -11280,7 +11280,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -11297,7 +11297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -11314,7 +11314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -11331,7 +11331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -11348,7 +11348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -11365,7 +11365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -11382,7 +11382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -11399,7 +11399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -11416,7 +11416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -11433,7 +11433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -11450,7 +11450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -11467,7 +11467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -11484,7 +11484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -11501,7 +11501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -11518,7 +11518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -11535,7 +11535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -11552,7 +11552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -11569,7 +11569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -11586,7 +11586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -11603,7 +11603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -11620,7 +11620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -11637,7 +11637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -11654,7 +11654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -11671,7 +11671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -11688,7 +11688,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -11705,7 +11705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -11722,7 +11722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -11739,7 +11739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -11756,7 +11756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -11773,7 +11773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -11790,7 +11790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -11819,14 +11819,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -11837,7 +11837,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>11</v>
       </c>
@@ -11848,7 +11848,7 @@
         <v>43477.417071759257</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>11</v>
       </c>
@@ -11859,7 +11859,7 @@
         <v>43477.418182870373</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>11</v>
       </c>
@@ -11870,7 +11870,7 @@
         <v>43477.420694444445</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>11</v>
       </c>
@@ -11881,7 +11881,7 @@
         <v>43477.459050925929</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>11</v>
       </c>
@@ -11892,7 +11892,7 @@
         <v>43477.460497685184</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>11</v>
       </c>
@@ -11903,7 +11903,7 @@
         <v>43477.461770833332</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>11</v>
       </c>
@@ -11914,7 +11914,7 @@
         <v>43478.544317129628</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>11</v>
       </c>
@@ -11925,7 +11925,7 @@
         <v>43478.552187499998</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>11</v>
       </c>
@@ -11936,7 +11936,7 @@
         <v>43478.594386574077</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>11</v>
       </c>
@@ -11947,7 +11947,7 @@
         <v>43478.596458333333</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -11958,7 +11958,7 @@
         <v>43478.628842592596</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -11969,7 +11969,7 @@
         <v>43478.636087962965</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -11980,7 +11980,7 @@
         <v>43482.754201388889</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>11</v>
       </c>
@@ -11991,7 +11991,7 @@
         <v>43484.417743055557</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>11</v>
       </c>
@@ -12002,7 +12002,7 @@
         <v>43484.422546296293</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>11</v>
       </c>
@@ -12013,7 +12013,7 @@
         <v>43484.42291666667</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>12</v>
       </c>
@@ -12024,7 +12024,7 @@
         <v>43484.426423611112</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>12</v>
       </c>
@@ -12035,7 +12035,7 @@
         <v>43484.431192129632</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>12</v>
       </c>
@@ -12046,7 +12046,7 @@
         <v>43484.43241898148</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>12</v>
       </c>
@@ -12057,7 +12057,7 @@
         <v>43484.434259259258</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>12</v>
       </c>
@@ -12068,7 +12068,7 @@
         <v>43484.460717592592</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>12</v>
       </c>
@@ -12079,7 +12079,7 @@
         <v>43484.462060185186</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>12</v>
       </c>
@@ -12090,7 +12090,7 @@
         <v>43484.462858796294</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>12</v>
       </c>
@@ -12101,7 +12101,7 @@
         <v>43484.466307870367</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>12</v>
       </c>
@@ -12112,7 +12112,7 @@
         <v>43484.470775462964</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>12</v>
       </c>
@@ -12123,7 +12123,7 @@
         <v>43484.475682870368</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>12</v>
       </c>
@@ -12134,7 +12134,7 @@
         <v>43484.481122685182</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>12</v>
       </c>
@@ -12145,7 +12145,7 @@
         <v>43484.545046296298</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>14</v>
       </c>
@@ -12156,7 +12156,7 @@
         <v>43484.547118055554</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>14</v>
       </c>
@@ -12167,7 +12167,7 @@
         <v>43484.548460648148</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>14</v>
       </c>
@@ -12178,7 +12178,7 @@
         <v>43484.551631944443</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>14</v>
       </c>
@@ -12189,7 +12189,7 @@
         <v>43484.552407407406</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>14</v>
       </c>
@@ -12200,7 +12200,7 @@
         <v>43484.557893518519</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>14</v>
       </c>
@@ -12211,7 +12211,7 @@
         <v>43484.561956018515</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>11</v>
       </c>
@@ -12222,7 +12222,7 @@
         <v>43485.547951388886</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>11</v>
       </c>
@@ -12233,7 +12233,7 @@
         <v>43485.553495370368</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>12</v>
       </c>
@@ -12244,7 +12244,7 @@
         <v>43485.5546875</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>12</v>
       </c>
@@ -12255,7 +12255,7 @@
         <v>43485.557916666665</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>12</v>
       </c>
@@ -12266,7 +12266,7 @@
         <v>43485.560243055559</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>12</v>
       </c>
@@ -12277,7 +12277,7 @@
         <v>43485.56453703704</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>12</v>
       </c>
@@ -12288,7 +12288,7 @@
         <v>43485.565057870372</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>12</v>
       </c>
@@ -12299,7 +12299,7 @@
         <v>43485.587997685187</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>12</v>
       </c>
@@ -12310,7 +12310,7 @@
         <v>43485.590127314812</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>12</v>
       </c>
@@ -12321,7 +12321,7 @@
         <v>43485.59578703704</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>12</v>
       </c>
@@ -12332,7 +12332,7 @@
         <v>43485.601377314815</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>12</v>
       </c>
@@ -12343,7 +12343,7 @@
         <v>43485.60664351852</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>12</v>
       </c>
@@ -12354,7 +12354,7 @@
         <v>43485.609884259262</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>14</v>
       </c>
@@ -12365,7 +12365,7 @@
         <v>43485.614710648151</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>14</v>
       </c>
@@ -12376,7 +12376,7 @@
         <v>43485.61791666667</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>14</v>
       </c>
@@ -12387,7 +12387,7 @@
         <v>43485.626550925925</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>14</v>
       </c>
@@ -12398,7 +12398,7 @@
         <v>43485.629050925927</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>14</v>
       </c>
@@ -12409,7 +12409,7 @@
         <v>43485.63449074074</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>14</v>
       </c>
@@ -12420,7 +12420,7 @@
         <v>43485.638425925928</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>16</v>
       </c>
@@ -12431,7 +12431,7 @@
         <v>43485.64303240741</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>16</v>
       </c>
@@ -12442,7 +12442,7 @@
         <v>43485.647696759261</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>16</v>
       </c>
@@ -12453,7 +12453,7 @@
         <v>43485.651388888888</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>16</v>
       </c>
@@ -12464,7 +12464,7 @@
         <v>43485.653807870367</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>16</v>
       </c>
@@ -12475,7 +12475,7 @@
         <v>43485.659224537034</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>16</v>
       </c>
@@ -12486,7 +12486,7 @@
         <v>43486.750844907408</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>14</v>
       </c>
@@ -12497,7 +12497,7 @@
         <v>43486.767256944448</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>11</v>
       </c>
@@ -12509,7 +12509,7 @@
       </c>
       <c r="E62" s="1"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>14</v>
       </c>
@@ -12520,7 +12520,7 @@
         <v>43488.751446759263</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>12</v>
       </c>
@@ -12531,7 +12531,7 @@
         <v>43489.75099537037</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>12</v>
       </c>
@@ -12542,7 +12542,7 @@
         <v>43490.792407407411</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>12</v>
       </c>
@@ -12553,7 +12553,7 @@
         <v>43491.416898148149</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>11</v>
       </c>
@@ -12564,7 +12564,7 @@
         <v>43491.423159722224</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>12</v>
       </c>
@@ -12575,7 +12575,7 @@
         <v>43491.428483796299</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>12</v>
       </c>
@@ -12586,7 +12586,7 @@
         <v>43491.433634259258</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>12</v>
       </c>
@@ -12597,7 +12597,7 @@
         <v>43491.443773148145</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>12</v>
       </c>
@@ -12608,7 +12608,7 @@
         <v>43491.460578703707</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>12</v>
       </c>
@@ -12619,7 +12619,7 @@
         <v>43491.466435185182</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>12</v>
       </c>
@@ -12630,7 +12630,7 @@
         <v>43491.466863425929</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>12</v>
       </c>
@@ -12641,7 +12641,7 @@
         <v>43491.469293981485</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>12</v>
       </c>
@@ -12652,7 +12652,7 @@
         <v>43491.471574074072</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>14</v>
       </c>
@@ -12663,7 +12663,7 @@
         <v>43491.472384259258</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>14</v>
       </c>
@@ -12674,7 +12674,7 @@
         <v>43491.547118055554</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>14</v>
       </c>
@@ -12685,7 +12685,7 @@
         <v>43491.548460648148</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>14</v>
       </c>
@@ -12696,7 +12696,7 @@
         <v>43491.553715277776</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>14</v>
       </c>
@@ -12707,7 +12707,7 @@
         <v>43491.558009259257</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>16</v>
       </c>
@@ -12718,7 +12718,7 @@
         <v>43491.562002314815</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>16</v>
       </c>
@@ -12729,7 +12729,7 @@
         <v>43491.565486111111</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>16</v>
       </c>
@@ -12740,7 +12740,7 @@
         <v>43491.56690972222</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>16</v>
       </c>
@@ -12751,7 +12751,7 @@
         <v>43491.569699074076</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>11</v>
       </c>
@@ -12762,7 +12762,7 @@
         <v>43492.546018518522</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>12</v>
       </c>
@@ -12773,7 +12773,7 @@
         <v>43492.549930555557</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>12</v>
       </c>
@@ -12784,7 +12784,7 @@
         <v>43492.552430555559</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>12</v>
       </c>
@@ -12795,7 +12795,7 @@
         <v>43492.555543981478</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>12</v>
       </c>
@@ -12806,7 +12806,7 @@
         <v>43492.556539351855</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>12</v>
       </c>
@@ -12817,7 +12817,7 @@
         <v>43492.586678240739</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>12</v>
       </c>
@@ -12828,7 +12828,7 @@
         <v>43492.587060185186</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>12</v>
       </c>
@@ -12839,7 +12839,7 @@
         <v>43492.591527777775</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>12</v>
       </c>
@@ -12850,7 +12850,7 @@
         <v>43492.595983796295</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>14</v>
       </c>
@@ -12861,7 +12861,7 @@
         <v>43492.597268518519</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>14</v>
       </c>
@@ -12872,7 +12872,7 @@
         <v>43492.630497685182</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>16</v>
       </c>
@@ -12883,7 +12883,7 @@
         <v>43492.634293981479</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>16</v>
       </c>
@@ -12894,7 +12894,7 @@
         <v>43492.636354166665</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>16</v>
       </c>
@@ -12905,7 +12905,7 @@
         <v>43492.643391203703</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>16</v>
       </c>
@@ -12916,7 +12916,7 @@
         <v>43492.644317129627</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>16</v>
       </c>
@@ -12927,7 +12927,7 @@
         <v>43493.731493055559</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>16</v>
       </c>
@@ -12938,7 +12938,7 @@
         <v>43493.735914351855</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>16</v>
       </c>
@@ -12949,7 +12949,7 @@
         <v>43493.739560185182</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>14</v>
       </c>
@@ -12960,7 +12960,7 @@
         <v>43495.751099537039</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>12</v>
       </c>
@@ -12971,7 +12971,7 @@
         <v>43495.761493055557</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>12</v>
       </c>
@@ -12982,7 +12982,7 @@
         <v>43496.751493055555</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>12</v>
       </c>
@@ -12993,7 +12993,7 @@
         <v>43497.796087962961</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>12</v>
       </c>
@@ -13004,7 +13004,7 @@
         <v>43497.797615740739</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>11</v>
       </c>
@@ -13015,7 +13015,7 @@
         <v>43498.418240740742</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>12</v>
       </c>
@@ -13026,7 +13026,7 @@
         <v>43498.423067129632</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>11</v>
       </c>
@@ -13037,7 +13037,7 @@
         <v>43498.427372685182</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>12</v>
       </c>
@@ -13048,7 +13048,7 @@
         <v>43498.462719907409</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>12</v>
       </c>
@@ -13059,7 +13059,7 @@
         <v>43498.465057870373</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>12</v>
       </c>
@@ -13070,7 +13070,7 @@
         <v>43498.467199074075</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>12</v>
       </c>
@@ -13081,7 +13081,7 @@
         <v>43498.545405092591</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>14</v>
       </c>
@@ -13092,7 +13092,7 @@
         <v>43498.550034722219</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>14</v>
       </c>
@@ -13103,7 +13103,7 @@
         <v>43498.550763888888</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>16</v>
       </c>
@@ -13114,7 +13114,7 @@
         <v>43498.556620370371</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>16</v>
       </c>
@@ -13125,7 +13125,7 @@
         <v>43498.557615740741</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>14</v>
       </c>
@@ -13136,7 +13136,7 @@
         <v>43499.543877314813</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>12</v>
       </c>
@@ -13147,7 +13147,7 @@
         <v>43499.544965277775</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>12</v>
       </c>
@@ -13158,7 +13158,7 @@
         <v>43499.546701388892</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>12</v>
       </c>
@@ -13169,7 +13169,7 @@
         <v>43499.586701388886</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>12</v>
       </c>
@@ -13180,7 +13180,7 @@
         <v>43499.587500000001</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>14</v>
       </c>
@@ -13191,7 +13191,7 @@
         <v>43499.590636574074</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>14</v>
       </c>
@@ -13202,7 +13202,7 @@
         <v>43499.632280092592</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>16</v>
       </c>
@@ -13213,7 +13213,7 @@
         <v>43499.635312500002</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>16</v>
       </c>
@@ -13237,23 +13237,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -13291,7 +13291,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -13314,7 +13314,7 @@
         <v>4389</v>
       </c>
       <c r="H2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="I2" t="s">
         <v>253</v>
@@ -13329,7 +13329,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -13352,10 +13352,10 @@
         <v>1707</v>
       </c>
       <c r="H3" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="I3" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="J3" t="s">
         <v>683</v>
@@ -13367,7 +13367,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -13390,7 +13390,7 @@
         <v>3107</v>
       </c>
       <c r="H4" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="I4" t="s">
         <v>687</v>
@@ -13405,7 +13405,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -13428,10 +13428,10 @@
         <v>1042</v>
       </c>
       <c r="H5" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="I5" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="J5" t="s">
         <v>683</v>
@@ -13443,12 +13443,12 @@
         <v>705</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C6">
         <v>16</v>
@@ -13466,10 +13466,10 @@
         <v>3389</v>
       </c>
       <c r="H6" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="I6" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="J6" t="s">
         <v>551</v>
@@ -13481,7 +13481,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -13504,10 +13504,10 @@
         <v>4472</v>
       </c>
       <c r="H7" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="I7" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="J7" t="s">
         <v>683</v>
@@ -13519,7 +13519,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -13542,7 +13542,7 @@
         <v>3957</v>
       </c>
       <c r="H8" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="I8" t="s">
         <v>691</v>
@@ -13557,7 +13557,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -13580,7 +13580,7 @@
         <v>3259</v>
       </c>
       <c r="H9" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="I9" t="s">
         <v>692</v>
@@ -13595,12 +13595,12 @@
         <v>708</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="C10">
         <v>12</v>
@@ -13618,10 +13618,10 @@
         <v>3283</v>
       </c>
       <c r="H10" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="I10" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="J10" t="s">
         <v>684</v>
@@ -13633,12 +13633,12 @@
         <v>709</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C11">
         <v>16</v>
@@ -13656,10 +13656,10 @@
         <v>2627</v>
       </c>
       <c r="H11" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="I11" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="J11" t="s">
         <v>684</v>
@@ -13671,12 +13671,12 @@
         <v>710</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C12">
         <v>14</v>
@@ -13694,10 +13694,10 @@
         <v>1283</v>
       </c>
       <c r="H12" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="I12" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="J12" t="s">
         <v>685</v>
@@ -13709,7 +13709,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -13732,7 +13732,7 @@
         <v>1888</v>
       </c>
       <c r="H13" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="I13" t="s">
         <v>695</v>
@@ -13747,7 +13747,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -13770,10 +13770,10 @@
         <v>4183</v>
       </c>
       <c r="H14" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="I14" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="J14" t="s">
         <v>683</v>
@@ -13785,12 +13785,12 @@
         <v>683</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C15">
         <v>12</v>
@@ -13808,10 +13808,10 @@
         <v>4430</v>
       </c>
       <c r="H15" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="I15" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="J15" t="s">
         <v>686</v>
@@ -13823,7 +13823,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -13846,10 +13846,10 @@
         <v>4598</v>
       </c>
       <c r="H16" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="I16" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="J16" t="s">
         <v>683</v>
@@ -13861,7 +13861,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -13884,10 +13884,10 @@
         <v>3639</v>
       </c>
       <c r="H17" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="I17" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="J17" t="s">
         <v>551</v>
@@ -13899,7 +13899,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -13922,7 +13922,7 @@
         <v>2937</v>
       </c>
       <c r="H18" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="I18" t="s">
         <v>701</v>

</xml_diff>

<commit_message>
Update prix/date vente null
</commit_message>
<xml_diff>
--- a/Jeu d'essai.xlsx
+++ b/Jeu d'essai.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="550" documentId="114_{8D9B191C-2013-4270-87A9-3FB899E57325}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{555E46CF-7038-4B79-8154-9B28D07E2385}"/>
+  <xr:revisionPtr revIDLastSave="566" documentId="114_{8D9B191C-2013-4270-87A9-3FB899E57325}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{175A67BF-E76D-446B-87C3-7623B42B2C40}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1765" uniqueCount="907">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1859" uniqueCount="907">
   <si>
     <t>NULL</t>
   </si>
@@ -5957,7 +5957,7 @@
   <sheetPr codeName="Feuil4"/>
   <dimension ref="A1:N132"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6050,11 +6050,11 @@
       <c r="I2" s="2">
         <v>1</v>
       </c>
-      <c r="J2" s="4">
-        <v>43532.999988425923</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>267</v>
+      <c r="J2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>112</v>
@@ -6094,11 +6094,11 @@
       <c r="I3" s="2">
         <v>1</v>
       </c>
-      <c r="J3" s="4">
-        <v>43533.999988425923</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>350</v>
+      <c r="J3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>115</v>
@@ -6138,11 +6138,11 @@
       <c r="I4" s="2">
         <v>1</v>
       </c>
-      <c r="J4" s="4">
-        <v>43533.999988425923</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>351</v>
+      <c r="J4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>122</v>
@@ -6182,11 +6182,11 @@
       <c r="I5" s="2">
         <v>1</v>
       </c>
-      <c r="J5" s="4">
-        <v>43533.999988425923</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>74</v>
+      <c r="J5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>119</v>
@@ -6226,11 +6226,11 @@
       <c r="I6" s="2">
         <v>1</v>
       </c>
-      <c r="J6" s="4">
-        <v>43533.999988425923</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>74</v>
+      <c r="J6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>115</v>
@@ -6270,11 +6270,11 @@
       <c r="I7" s="6">
         <v>1</v>
       </c>
-      <c r="J7" s="4">
-        <v>43533.999988425923</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>352</v>
+      <c r="J7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>149</v>
@@ -6317,7 +6317,7 @@
       <c r="J8" s="4">
         <v>43534.999988368058</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="2" t="s">
         <v>353</v>
       </c>
       <c r="L8" s="2" t="s">
@@ -6361,7 +6361,7 @@
       <c r="J9" s="4">
         <v>43534.999988368058</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="K9" s="2" t="s">
         <v>670</v>
       </c>
       <c r="L9" s="2" t="s">
@@ -6405,7 +6405,7 @@
       <c r="J10" s="4">
         <v>43534.999988368058</v>
       </c>
-      <c r="K10" s="6" t="s">
+      <c r="K10" s="2" t="s">
         <v>418</v>
       </c>
       <c r="L10" s="2" t="s">
@@ -6446,11 +6446,11 @@
       <c r="I11" s="6">
         <v>1</v>
       </c>
-      <c r="J11" s="4">
-        <v>43535.999988368058</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>468</v>
+      <c r="J11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>137</v>
@@ -6490,11 +6490,11 @@
       <c r="I12" s="6">
         <v>1</v>
       </c>
-      <c r="J12" s="4">
-        <v>43535.999988368058</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>471</v>
+      <c r="J12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>460</v>
@@ -6534,11 +6534,11 @@
       <c r="I13" s="6">
         <v>1</v>
       </c>
-      <c r="J13" s="4">
-        <v>43535.999988368058</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>475</v>
+      <c r="J13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>474</v>
@@ -6578,11 +6578,11 @@
       <c r="I14" s="6">
         <v>1</v>
       </c>
-      <c r="J14" s="4">
-        <v>43535.999988368058</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>477</v>
+      <c r="J14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>203</v>
@@ -6622,11 +6622,11 @@
       <c r="I15" s="6">
         <v>1</v>
       </c>
-      <c r="J15" s="4">
-        <v>43536.999988368058</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>348</v>
+      <c r="J15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>508</v>
@@ -6666,11 +6666,11 @@
       <c r="I16" s="6">
         <v>1</v>
       </c>
-      <c r="J16" s="4">
-        <v>43536.999988368058</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>398</v>
+      <c r="J16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>511</v>
@@ -6710,11 +6710,11 @@
       <c r="I17" s="6">
         <v>1</v>
       </c>
-      <c r="J17" s="4">
-        <v>43536.999988368058</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>533</v>
+      <c r="J17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>534</v>
@@ -6754,11 +6754,11 @@
       <c r="I18" s="6">
         <v>1</v>
       </c>
-      <c r="J18" s="4">
-        <v>43536.999988368058</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>517</v>
+      <c r="J18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>137</v>
@@ -6798,11 +6798,11 @@
       <c r="I19" s="6">
         <v>0</v>
       </c>
-      <c r="J19" s="4">
-        <v>43536.999988368058</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>253</v>
+      <c r="J19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>521</v>
@@ -6842,11 +6842,11 @@
       <c r="I20" s="6">
         <v>1</v>
       </c>
-      <c r="J20" s="4">
-        <v>43536.999988368058</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>525</v>
+      <c r="J20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>526</v>
@@ -6886,11 +6886,11 @@
       <c r="I21" s="6">
         <v>1</v>
       </c>
-      <c r="J21" s="4">
-        <v>43536.999988368058</v>
-      </c>
-      <c r="K21" s="6" t="s">
-        <v>529</v>
+      <c r="J21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>474</v>
@@ -6930,11 +6930,11 @@
       <c r="I22" s="6">
         <v>1</v>
       </c>
-      <c r="J22" s="4">
-        <v>43536.999988368058</v>
-      </c>
-      <c r="K22" s="6" t="s">
-        <v>538</v>
+      <c r="J22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>539</v>
@@ -6974,11 +6974,11 @@
       <c r="I23" s="6">
         <v>1</v>
       </c>
-      <c r="J23" s="4">
-        <v>43536.999988368058</v>
-      </c>
-      <c r="K23" s="6" t="s">
-        <v>542</v>
+      <c r="J23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>134</v>
@@ -7018,11 +7018,11 @@
       <c r="I24" s="6">
         <v>1</v>
       </c>
-      <c r="J24" s="4">
-        <v>43536.999988368058</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>545</v>
+      <c r="J24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>547</v>
@@ -7062,11 +7062,11 @@
       <c r="I25" s="6">
         <v>0</v>
       </c>
-      <c r="J25" s="4">
-        <v>43536.999988368058</v>
-      </c>
-      <c r="K25" s="6" t="s">
-        <v>550</v>
+      <c r="J25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>552</v>
@@ -7106,11 +7106,11 @@
       <c r="I26" s="6">
         <v>1</v>
       </c>
-      <c r="J26" s="4">
-        <v>43536.999988368058</v>
-      </c>
-      <c r="K26" s="6" t="s">
-        <v>555</v>
+      <c r="J26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>556</v>
@@ -7150,11 +7150,11 @@
       <c r="I27" s="6">
         <v>1</v>
       </c>
-      <c r="J27" s="4">
-        <v>43536.999988368058</v>
-      </c>
-      <c r="K27" s="6" t="s">
-        <v>561</v>
+      <c r="J27" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>562</v>
@@ -7194,11 +7194,11 @@
       <c r="I28" s="6">
         <v>1</v>
       </c>
-      <c r="J28" s="4">
-        <v>43536.999988368058</v>
-      </c>
-      <c r="K28" s="6" t="s">
-        <v>550</v>
+      <c r="J28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>552</v>
@@ -7238,11 +7238,11 @@
       <c r="I29" s="6">
         <v>1</v>
       </c>
-      <c r="J29" s="4">
-        <v>43537.999988368058</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>352</v>
+      <c r="J29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>106</v>
@@ -7282,11 +7282,11 @@
       <c r="I30" s="6">
         <v>1</v>
       </c>
-      <c r="J30" s="4">
-        <v>43537.999988368058</v>
-      </c>
-      <c r="K30" s="6" t="s">
-        <v>356</v>
+      <c r="J30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>116</v>
@@ -7326,11 +7326,11 @@
       <c r="I31" s="6">
         <v>0</v>
       </c>
-      <c r="J31" s="4">
-        <v>43537.999988368058</v>
-      </c>
-      <c r="K31" s="6" t="s">
-        <v>359</v>
+      <c r="J31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L31" s="2" t="s">
         <v>118</v>
@@ -7370,11 +7370,11 @@
       <c r="I32" s="6">
         <v>1</v>
       </c>
-      <c r="J32" s="4">
-        <v>43538.999988368058</v>
-      </c>
-      <c r="K32" s="6" t="s">
-        <v>607</v>
+      <c r="J32" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L32" s="2" t="s">
         <v>608</v>
@@ -7414,11 +7414,11 @@
       <c r="I33" s="6">
         <v>1</v>
       </c>
-      <c r="J33" s="4">
-        <v>43538.999988368058</v>
-      </c>
-      <c r="K33" s="6" t="s">
-        <v>612</v>
+      <c r="J33" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L33" s="2" t="s">
         <v>562</v>
@@ -7458,11 +7458,11 @@
       <c r="I34" s="6">
         <v>1</v>
       </c>
-      <c r="J34" s="4">
-        <v>43539.999988368058</v>
-      </c>
-      <c r="K34" s="6" t="s">
-        <v>345</v>
+      <c r="J34" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>207</v>
@@ -7502,11 +7502,11 @@
       <c r="I35" s="6">
         <v>1</v>
       </c>
-      <c r="J35" s="4">
-        <v>43539.999988368058</v>
-      </c>
-      <c r="K35" s="6" t="s">
-        <v>210</v>
+      <c r="J35" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L35" s="2" t="s">
         <v>116</v>
@@ -7546,11 +7546,11 @@
       <c r="I36" s="6">
         <v>1</v>
       </c>
-      <c r="J36" s="4">
-        <v>43539.999988368058</v>
-      </c>
-      <c r="K36" s="6" t="s">
-        <v>215</v>
+      <c r="J36" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L36" s="2" t="s">
         <v>214</v>
@@ -7590,11 +7590,11 @@
       <c r="I37" s="6">
         <v>1</v>
       </c>
-      <c r="J37" s="4">
-        <v>43539.999988368058</v>
-      </c>
-      <c r="K37" s="6" t="s">
-        <v>346</v>
+      <c r="J37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>219</v>
@@ -7634,11 +7634,11 @@
       <c r="I38" s="6">
         <v>1</v>
       </c>
-      <c r="J38" s="4">
-        <v>43539.999988368058</v>
-      </c>
-      <c r="K38" s="6" t="s">
-        <v>347</v>
+      <c r="J38" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L38" s="2" t="s">
         <v>223</v>
@@ -7678,11 +7678,11 @@
       <c r="I39" s="6">
         <v>1</v>
       </c>
-      <c r="J39" s="4">
-        <v>43539.999988368058</v>
-      </c>
-      <c r="K39" s="6" t="s">
-        <v>373</v>
+      <c r="J39" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L39" s="2" t="s">
         <v>374</v>
@@ -7722,11 +7722,11 @@
       <c r="I40" s="6">
         <v>1</v>
       </c>
-      <c r="J40" s="4">
-        <v>43539.999988368058</v>
-      </c>
-      <c r="K40" s="6" t="s">
-        <v>377</v>
+      <c r="J40" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L40" s="2" t="s">
         <v>378</v>
@@ -7766,11 +7766,11 @@
       <c r="I41" s="6">
         <v>1</v>
       </c>
-      <c r="J41" s="4">
-        <v>43539.999988368058</v>
-      </c>
-      <c r="K41" s="6" t="s">
-        <v>381</v>
+      <c r="J41" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L41" s="2" t="s">
         <v>382</v>
@@ -7810,11 +7810,11 @@
       <c r="I42" s="6">
         <v>1</v>
       </c>
-      <c r="J42" s="4">
-        <v>43539.999988368058</v>
-      </c>
-      <c r="K42" s="6" t="s">
-        <v>385</v>
+      <c r="J42" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L42" s="2" t="s">
         <v>386</v>
@@ -7854,11 +7854,11 @@
       <c r="I43" s="6">
         <v>1</v>
       </c>
-      <c r="J43" s="4">
-        <v>43539.999988368058</v>
-      </c>
-      <c r="K43" s="6" t="s">
-        <v>389</v>
+      <c r="J43" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L43" s="2" t="s">
         <v>390</v>
@@ -7898,11 +7898,11 @@
       <c r="I44" s="6">
         <v>1</v>
       </c>
-      <c r="J44" s="4">
-        <v>43539.999988368058</v>
-      </c>
-      <c r="K44" s="6" t="s">
-        <v>394</v>
+      <c r="J44" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L44" s="2" t="s">
         <v>393</v>
@@ -7942,11 +7942,11 @@
       <c r="I45" s="6">
         <v>0</v>
       </c>
-      <c r="J45" s="4">
-        <v>43539.999988368058</v>
-      </c>
-      <c r="K45" s="6" t="s">
-        <v>398</v>
+      <c r="J45" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L45" s="2" t="s">
         <v>399</v>
@@ -7986,11 +7986,11 @@
       <c r="I46" s="6">
         <v>1</v>
       </c>
-      <c r="J46" s="4">
-        <v>43539.999988368058</v>
-      </c>
-      <c r="K46" s="6" t="s">
-        <v>402</v>
+      <c r="J46" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L46" s="2" t="s">
         <v>325</v>
@@ -8030,11 +8030,11 @@
       <c r="I47" s="6">
         <v>0</v>
       </c>
-      <c r="J47" s="4">
-        <v>43540.999988368058</v>
-      </c>
-      <c r="K47" s="6" t="s">
-        <v>342</v>
+      <c r="J47" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L47" s="2" t="s">
         <v>131</v>
@@ -8074,11 +8074,11 @@
       <c r="I48" s="6">
         <v>1</v>
       </c>
-      <c r="J48" s="4">
-        <v>43540.999988368058</v>
-      </c>
-      <c r="K48" s="6" t="s">
-        <v>342</v>
+      <c r="J48" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L48" s="2" t="s">
         <v>134</v>
@@ -8118,11 +8118,11 @@
       <c r="I49" s="6">
         <v>1</v>
       </c>
-      <c r="J49" s="4">
-        <v>43540.999988368058</v>
-      </c>
-      <c r="K49" s="6" t="s">
-        <v>343</v>
+      <c r="J49" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L49" s="2" t="s">
         <v>407</v>
@@ -8162,11 +8162,11 @@
       <c r="I50" s="6">
         <v>1</v>
       </c>
-      <c r="J50" s="4">
-        <v>43541.999988368058</v>
-      </c>
-      <c r="K50" s="6" t="s">
-        <v>354</v>
+      <c r="J50" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L50" s="2" t="s">
         <v>156</v>
@@ -8206,11 +8206,11 @@
       <c r="I51" s="6">
         <v>1</v>
       </c>
-      <c r="J51" s="4">
-        <v>43541.999988368058</v>
-      </c>
-      <c r="K51" s="6" t="s">
-        <v>355</v>
+      <c r="J51" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L51" s="2" t="s">
         <v>115</v>
@@ -8250,11 +8250,11 @@
       <c r="I52" s="6">
         <v>1</v>
       </c>
-      <c r="J52" s="4">
-        <v>43541.999988368058</v>
-      </c>
-      <c r="K52" s="6" t="s">
-        <v>352</v>
+      <c r="J52" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L52" s="2" t="s">
         <v>161</v>
@@ -8294,11 +8294,11 @@
       <c r="I53" s="6">
         <v>1</v>
       </c>
-      <c r="J53" s="4">
-        <v>43541.999988368058</v>
-      </c>
-      <c r="K53" s="6" t="s">
-        <v>253</v>
+      <c r="J53" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L53" s="2" t="s">
         <v>106</v>
@@ -8338,11 +8338,11 @@
       <c r="I54" s="6">
         <v>1</v>
       </c>
-      <c r="J54" s="4">
-        <v>43542.999988368058</v>
-      </c>
-      <c r="K54" s="6" t="s">
-        <v>350</v>
+      <c r="J54" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L54" s="2" t="s">
         <v>164</v>
@@ -8382,11 +8382,11 @@
       <c r="I55" s="6">
         <v>1</v>
       </c>
-      <c r="J55" s="4">
-        <v>43542.999988368058</v>
-      </c>
-      <c r="K55" s="6" t="s">
-        <v>267</v>
+      <c r="J55" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L55" s="2" t="s">
         <v>167</v>
@@ -8426,11 +8426,11 @@
       <c r="I56" s="6">
         <v>1</v>
       </c>
-      <c r="J56" s="4">
-        <v>43542.999988368058</v>
-      </c>
-      <c r="K56" s="6" t="s">
-        <v>357</v>
+      <c r="J56" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L56" s="2" t="s">
         <v>169</v>
@@ -8470,11 +8470,11 @@
       <c r="I57" s="6">
         <v>1</v>
       </c>
-      <c r="J57" s="4">
-        <v>43542.999988368058</v>
-      </c>
-      <c r="K57" s="6" t="s">
-        <v>342</v>
+      <c r="J57" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K57" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L57" s="2" t="s">
         <v>149</v>
@@ -8514,11 +8514,11 @@
       <c r="I58" s="6">
         <v>1</v>
       </c>
-      <c r="J58" s="4">
-        <v>43542.999988368058</v>
-      </c>
-      <c r="K58" s="6" t="s">
-        <v>358</v>
+      <c r="J58" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K58" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L58" s="2" t="s">
         <v>137</v>
@@ -8558,11 +8558,11 @@
       <c r="I59" s="6">
         <v>1</v>
       </c>
-      <c r="J59" s="4">
-        <v>43542.999988368058</v>
-      </c>
-      <c r="K59" s="6" t="s">
-        <v>568</v>
+      <c r="J59" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K59" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L59" s="2" t="s">
         <v>137</v>
@@ -8602,11 +8602,11 @@
       <c r="I60" s="6">
         <v>1</v>
       </c>
-      <c r="J60" s="4">
-        <v>43543.999988368058</v>
-      </c>
-      <c r="K60" s="6" t="s">
-        <v>617</v>
+      <c r="J60" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L60" s="2" t="s">
         <v>618</v>
@@ -8646,11 +8646,11 @@
       <c r="I61" s="6">
         <v>1</v>
       </c>
-      <c r="J61" s="4">
-        <v>43543.999988368058</v>
-      </c>
-      <c r="K61" s="6" t="s">
-        <v>622</v>
+      <c r="J61" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K61" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L61" s="2" t="s">
         <v>624</v>
@@ -8690,11 +8690,11 @@
       <c r="I62" s="6">
         <v>1</v>
       </c>
-      <c r="J62" s="4">
-        <v>43543.999988368058</v>
-      </c>
-      <c r="K62" s="6" t="s">
-        <v>627</v>
+      <c r="J62" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K62" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L62" s="2" t="s">
         <v>618</v>
@@ -8734,11 +8734,11 @@
       <c r="I63" s="6">
         <v>1</v>
       </c>
-      <c r="J63" s="4">
-        <v>43543.999988368058</v>
-      </c>
-      <c r="K63" s="6" t="s">
-        <v>632</v>
+      <c r="J63" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K63" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L63" s="2" t="s">
         <v>633</v>
@@ -8778,11 +8778,11 @@
       <c r="I64" s="6">
         <v>0</v>
       </c>
-      <c r="J64" s="4">
-        <v>43543.999988368058</v>
-      </c>
-      <c r="K64" s="6" t="s">
-        <v>637</v>
+      <c r="J64" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K64" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L64" s="2" t="s">
         <v>188</v>
@@ -8822,11 +8822,11 @@
       <c r="I65" s="6">
         <v>1</v>
       </c>
-      <c r="J65" s="4">
-        <v>43543.999988368058</v>
-      </c>
-      <c r="K65" s="6" t="s">
-        <v>641</v>
+      <c r="J65" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K65" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L65" s="2" t="s">
         <v>464</v>
@@ -8869,7 +8869,7 @@
       <c r="J66" s="4">
         <v>43544.999988368058</v>
       </c>
-      <c r="K66" s="6" t="s">
+      <c r="K66" s="2" t="s">
         <v>666</v>
       </c>
       <c r="L66" s="2" t="s">
@@ -8913,7 +8913,7 @@
       <c r="J67" s="4">
         <v>43544.999988368058</v>
       </c>
-      <c r="K67" s="6" t="s">
+      <c r="K67" s="2" t="s">
         <v>182</v>
       </c>
       <c r="L67" s="2" t="s">
@@ -8957,7 +8957,7 @@
       <c r="J68" s="4">
         <v>43544.999988368058</v>
       </c>
-      <c r="K68" s="6" t="s">
+      <c r="K68" s="2" t="s">
         <v>667</v>
       </c>
       <c r="L68" s="2" t="s">
@@ -9001,7 +9001,7 @@
       <c r="J69" s="4">
         <v>43544.999988368058</v>
       </c>
-      <c r="K69" s="6" t="s">
+      <c r="K69" s="2" t="s">
         <v>468</v>
       </c>
       <c r="L69" s="2" t="s">
@@ -9045,7 +9045,7 @@
       <c r="J70" s="4">
         <v>43544.999988368058</v>
       </c>
-      <c r="K70" s="6" t="s">
+      <c r="K70" s="2" t="s">
         <v>668</v>
       </c>
       <c r="L70" s="2" t="s">
@@ -9089,7 +9089,7 @@
       <c r="J71" s="4">
         <v>43544.999988368058</v>
       </c>
-      <c r="K71" s="6" t="s">
+      <c r="K71" s="2" t="s">
         <v>555</v>
       </c>
       <c r="L71" s="2" t="s">
@@ -9133,7 +9133,7 @@
       <c r="J72" s="4">
         <v>43544.999988368058</v>
       </c>
-      <c r="K72" s="6" t="s">
+      <c r="K72" s="2" t="s">
         <v>669</v>
       </c>
       <c r="L72" s="2" t="s">
@@ -9174,11 +9174,11 @@
       <c r="I73" s="6">
         <v>1</v>
       </c>
-      <c r="J73" s="4">
-        <v>43545.999988368058</v>
-      </c>
-      <c r="K73" s="6" t="s">
-        <v>253</v>
+      <c r="J73" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K73" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L73" s="2" t="s">
         <v>128</v>
@@ -9218,11 +9218,11 @@
       <c r="I74" s="6">
         <v>1</v>
       </c>
-      <c r="J74" s="4">
-        <v>43545.999988368058</v>
-      </c>
-      <c r="K74" s="6" t="s">
-        <v>181</v>
+      <c r="J74" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K74" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L74" s="2" t="s">
         <v>183</v>
@@ -9262,11 +9262,11 @@
       <c r="I75" s="6">
         <v>1</v>
       </c>
-      <c r="J75" s="4">
-        <v>43545.999988368058</v>
-      </c>
-      <c r="K75" s="6" t="s">
-        <v>343</v>
+      <c r="J75" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K75" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L75" s="2" t="s">
         <v>140</v>
@@ -9306,11 +9306,11 @@
       <c r="I76" s="6">
         <v>1</v>
       </c>
-      <c r="J76" s="4">
-        <v>43545.999988368058</v>
-      </c>
-      <c r="K76" s="6" t="s">
-        <v>344</v>
+      <c r="J76" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K76" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L76" s="2" t="s">
         <v>143</v>
@@ -9350,11 +9350,11 @@
       <c r="I77" s="6">
         <v>1</v>
       </c>
-      <c r="J77" s="4">
-        <v>43545.999988368058</v>
-      </c>
-      <c r="K77" s="6" t="s">
-        <v>260</v>
+      <c r="J77" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K77" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L77" s="2" t="s">
         <v>146</v>
@@ -9394,11 +9394,11 @@
       <c r="I78" s="6">
         <v>1</v>
       </c>
-      <c r="J78" s="4">
-        <v>43545.999988368058</v>
-      </c>
-      <c r="K78" s="6" t="s">
-        <v>196</v>
+      <c r="J78" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K78" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L78" s="2" t="s">
         <v>197</v>
@@ -9438,11 +9438,11 @@
       <c r="I79" s="6">
         <v>1</v>
       </c>
-      <c r="J79" s="4">
-        <v>43546.999988368058</v>
-      </c>
-      <c r="K79" s="6" t="s">
-        <v>353</v>
+      <c r="J79" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K79" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L79" s="2" t="s">
         <v>137</v>
@@ -9482,11 +9482,11 @@
       <c r="I80" s="6">
         <v>1</v>
       </c>
-      <c r="J80" s="4">
-        <v>43546.999988368058</v>
-      </c>
-      <c r="K80" s="6" t="s">
-        <v>267</v>
+      <c r="J80" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K80" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L80" s="2" t="s">
         <v>137</v>
@@ -9526,11 +9526,11 @@
       <c r="I81" s="6">
         <v>1</v>
       </c>
-      <c r="J81" s="4">
-        <v>43546.999988368058</v>
-      </c>
-      <c r="K81" s="6" t="s">
-        <v>364</v>
+      <c r="J81" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K81" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L81" s="2" t="s">
         <v>325</v>
@@ -9570,11 +9570,11 @@
       <c r="I82" s="6">
         <v>1</v>
       </c>
-      <c r="J82" s="4">
-        <v>43546.999988368058</v>
-      </c>
-      <c r="K82" s="6" t="s">
-        <v>363</v>
+      <c r="J82" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K82" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L82" s="2" t="s">
         <v>134</v>
@@ -9614,11 +9614,11 @@
       <c r="I83" s="6">
         <v>1</v>
       </c>
-      <c r="J83" s="4">
-        <v>43547.999988368058</v>
-      </c>
-      <c r="K83" s="6" t="s">
-        <v>432</v>
+      <c r="J83" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K83" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L83" s="2" t="s">
         <v>336</v>
@@ -9658,11 +9658,11 @@
       <c r="I84" s="6">
         <v>1</v>
       </c>
-      <c r="J84" s="4">
-        <v>43547.999988368058</v>
-      </c>
-      <c r="K84" s="6" t="s">
-        <v>438</v>
+      <c r="J84" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K84" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L84" s="2" t="s">
         <v>437</v>
@@ -9702,11 +9702,11 @@
       <c r="I85" s="6">
         <v>1</v>
       </c>
-      <c r="J85" s="4">
-        <v>43547.999988368058</v>
-      </c>
-      <c r="K85" s="6" t="s">
-        <v>443</v>
+      <c r="J85" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K85" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L85" s="2" t="s">
         <v>441</v>
@@ -9746,11 +9746,11 @@
       <c r="I86" s="6">
         <v>1</v>
       </c>
-      <c r="J86" s="4">
-        <v>43547.999988368058</v>
-      </c>
-      <c r="K86" s="6" t="s">
-        <v>448</v>
+      <c r="J86" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K86" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L86" s="2" t="s">
         <v>446</v>
@@ -9790,11 +9790,11 @@
       <c r="I87" s="6">
         <v>1</v>
       </c>
-      <c r="J87" s="4">
-        <v>43547.999988368058</v>
-      </c>
-      <c r="K87" s="6" t="s">
-        <v>182</v>
+      <c r="J87" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K87" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L87" s="2" t="s">
         <v>393</v>
@@ -9834,11 +9834,11 @@
       <c r="I88" s="6">
         <v>1</v>
       </c>
-      <c r="J88" s="4">
-        <v>43547.999988368058</v>
-      </c>
-      <c r="K88" s="6" t="s">
-        <v>455</v>
+      <c r="J88" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K88" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L88" s="2" t="s">
         <v>454</v>
@@ -9878,11 +9878,11 @@
       <c r="I89" s="6">
         <v>1</v>
       </c>
-      <c r="J89" s="4">
-        <v>43547.999988368058</v>
-      </c>
-      <c r="K89" s="6" t="s">
-        <v>461</v>
+      <c r="J89" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K89" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L89" s="2" t="s">
         <v>460</v>
@@ -9922,11 +9922,11 @@
       <c r="I90" s="6">
         <v>1</v>
       </c>
-      <c r="J90" s="4">
-        <v>43547.999988368058</v>
-      </c>
-      <c r="K90" s="6" t="s">
-        <v>182</v>
+      <c r="J90" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K90" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L90" s="2" t="s">
         <v>464</v>
@@ -9966,11 +9966,11 @@
       <c r="I91" s="6">
         <v>1</v>
       </c>
-      <c r="J91" s="4">
-        <v>43548.999988368058</v>
-      </c>
-      <c r="K91" s="6" t="s">
-        <v>504</v>
+      <c r="J91" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K91" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L91" s="2" t="s">
         <v>137</v>
@@ -10010,11 +10010,11 @@
       <c r="I92" s="6">
         <v>1</v>
       </c>
-      <c r="J92" s="4">
-        <v>43548.999988368058</v>
-      </c>
-      <c r="K92" s="6" t="s">
-        <v>480</v>
+      <c r="J92" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K92" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L92" s="2" t="s">
         <v>325</v>
@@ -10054,11 +10054,11 @@
       <c r="I93" s="6">
         <v>1</v>
       </c>
-      <c r="J93" s="4">
-        <v>43548.999988368058</v>
-      </c>
-      <c r="K93" s="6" t="s">
-        <v>484</v>
+      <c r="J93" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K93" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L93" s="2" t="s">
         <v>325</v>
@@ -10098,11 +10098,11 @@
       <c r="I94" s="6">
         <v>1</v>
       </c>
-      <c r="J94" s="4">
-        <v>43548.999988368058</v>
-      </c>
-      <c r="K94" s="6" t="s">
-        <v>488</v>
+      <c r="J94" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K94" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L94" s="2" t="s">
         <v>137</v>
@@ -10142,11 +10142,11 @@
       <c r="I95" s="6">
         <v>1</v>
       </c>
-      <c r="J95" s="4">
-        <v>43548.999988368058</v>
-      </c>
-      <c r="K95" s="6" t="s">
-        <v>492</v>
+      <c r="J95" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K95" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L95" s="2" t="s">
         <v>325</v>
@@ -10186,11 +10186,11 @@
       <c r="I96" s="6">
         <v>1</v>
       </c>
-      <c r="J96" s="4">
-        <v>43548.999988368058</v>
-      </c>
-      <c r="K96" s="6" t="s">
-        <v>496</v>
+      <c r="J96" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K96" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L96" s="2" t="s">
         <v>325</v>
@@ -10230,11 +10230,11 @@
       <c r="I97" s="6">
         <v>1</v>
       </c>
-      <c r="J97" s="4">
-        <v>43548.999988368058</v>
-      </c>
-      <c r="K97" s="6" t="s">
-        <v>500</v>
+      <c r="J97" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K97" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L97" s="2" t="s">
         <v>325</v>
@@ -10274,11 +10274,11 @@
       <c r="I98" s="6">
         <v>1</v>
       </c>
-      <c r="J98" s="4">
-        <v>43549.999988368058</v>
-      </c>
-      <c r="K98" s="6" t="s">
-        <v>176</v>
+      <c r="J98" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K98" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L98" s="2" t="s">
         <v>188</v>
@@ -10318,11 +10318,11 @@
       <c r="I99" s="6">
         <v>1</v>
       </c>
-      <c r="J99" s="4">
-        <v>43549.999988368058</v>
-      </c>
-      <c r="K99" s="6" t="s">
-        <v>575</v>
+      <c r="J99" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K99" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L99" s="2" t="s">
         <v>577</v>
@@ -10362,11 +10362,11 @@
       <c r="I100" s="6">
         <v>1</v>
       </c>
-      <c r="J100" s="4">
-        <v>43549.999988368058</v>
-      </c>
-      <c r="K100" s="6" t="s">
-        <v>432</v>
+      <c r="J100" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K100" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L100" s="2" t="s">
         <v>586</v>
@@ -10406,11 +10406,11 @@
       <c r="I101" s="6">
         <v>1</v>
       </c>
-      <c r="J101" s="4">
-        <v>43549.999988368058</v>
-      </c>
-      <c r="K101" s="6" t="s">
-        <v>210</v>
+      <c r="J101" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K101" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="L101" s="2" t="s">
         <v>137</v>
@@ -10450,11 +10450,11 @@
       <c r="I102" s="2">
         <v>1</v>
       </c>
-      <c r="J102" s="4">
-        <v>43550.999988368058</v>
+      <c r="J102" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>589</v>
+        <v>0</v>
       </c>
       <c r="L102" s="2" t="s">
         <v>590</v>
@@ -10494,11 +10494,11 @@
       <c r="I103" s="2">
         <v>1</v>
       </c>
-      <c r="J103" s="4">
-        <v>43550.999988368058</v>
+      <c r="J103" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="K103" s="2" t="s">
-        <v>418</v>
+        <v>0</v>
       </c>
       <c r="L103" s="2" t="s">
         <v>115</v>
@@ -10538,11 +10538,11 @@
       <c r="I104" s="2">
         <v>1</v>
       </c>
-      <c r="J104" s="4">
-        <v>43550.999988368058</v>
+      <c r="J104" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="K104" s="2" t="s">
-        <v>602</v>
+        <v>0</v>
       </c>
       <c r="L104" s="2" t="s">
         <v>603</v>
@@ -10582,11 +10582,11 @@
       <c r="I105" s="2">
         <v>1</v>
       </c>
-      <c r="J105" s="4">
-        <v>43551.999988368058</v>
+      <c r="J105" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="K105" s="2" t="s">
-        <v>644</v>
+        <v>0</v>
       </c>
       <c r="L105" s="2" t="s">
         <v>460</v>
@@ -10626,10 +10626,10 @@
       <c r="I106" s="2">
         <v>1</v>
       </c>
-      <c r="J106" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K106" s="5" t="s">
+      <c r="J106" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K106" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L106" s="2" t="s">
@@ -10670,10 +10670,10 @@
       <c r="I107" s="2">
         <v>1</v>
       </c>
-      <c r="J107" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K107" s="5" t="s">
+      <c r="J107" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K107" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L107" s="2" t="s">
@@ -10714,10 +10714,10 @@
       <c r="I108" s="2">
         <v>1</v>
       </c>
-      <c r="J108" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K108" s="5" t="s">
+      <c r="J108" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K108" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L108" s="2" t="s">
@@ -10758,10 +10758,10 @@
       <c r="I109" s="2">
         <v>1</v>
       </c>
-      <c r="J109" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K109" s="5" t="s">
+      <c r="J109" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K109" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L109" s="2" t="s">
@@ -10802,10 +10802,10 @@
       <c r="I110" s="2">
         <v>1</v>
       </c>
-      <c r="J110" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K110" s="5" t="s">
+      <c r="J110" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K110" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L110" s="2" t="s">
@@ -10846,10 +10846,10 @@
       <c r="I111" s="2">
         <v>1</v>
       </c>
-      <c r="J111" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K111" s="5" t="s">
+      <c r="J111" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K111" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L111" s="2" t="s">
@@ -10890,10 +10890,10 @@
       <c r="I112" s="2">
         <v>1</v>
       </c>
-      <c r="J112" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K112" s="5" t="s">
+      <c r="J112" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K112" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L112" s="2" t="s">
@@ -10934,10 +10934,10 @@
       <c r="I113" s="2">
         <v>1</v>
       </c>
-      <c r="J113" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K113" s="5" t="s">
+      <c r="J113" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K113" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L113" s="2" t="s">
@@ -11066,10 +11066,10 @@
       <c r="I116" s="2">
         <v>1</v>
       </c>
-      <c r="J116" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K116" s="5" t="s">
+      <c r="J116" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K116" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L116" s="2" t="s">
@@ -11110,10 +11110,10 @@
       <c r="I117" s="2">
         <v>1</v>
       </c>
-      <c r="J117" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K117" s="5" t="s">
+      <c r="J117" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K117" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L117" s="2" t="s">
@@ -11154,10 +11154,10 @@
       <c r="I118" s="2">
         <v>0</v>
       </c>
-      <c r="J118" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K118" s="5" t="s">
+      <c r="J118" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K118" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L118" s="2" t="s">
@@ -11198,10 +11198,10 @@
       <c r="I119" s="2">
         <v>1</v>
       </c>
-      <c r="J119" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K119" s="5" t="s">
+      <c r="J119" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K119" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L119" s="2" t="s">
@@ -11242,10 +11242,10 @@
       <c r="I120" s="2">
         <v>1</v>
       </c>
-      <c r="J120" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K120" s="5" t="s">
+      <c r="J120" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K120" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L120" s="2" t="s">
@@ -11286,10 +11286,10 @@
       <c r="I121" s="2">
         <v>1</v>
       </c>
-      <c r="J121" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K121" s="5" t="s">
+      <c r="J121" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K121" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L121" s="2" t="s">
@@ -11330,10 +11330,10 @@
       <c r="I122" s="2">
         <v>1</v>
       </c>
-      <c r="J122" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K122" s="5" t="s">
+      <c r="J122" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K122" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L122" s="2" t="s">
@@ -11374,10 +11374,10 @@
       <c r="I123" s="2">
         <v>1</v>
       </c>
-      <c r="J123" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K123" s="5" t="s">
+      <c r="J123" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K123" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L123" s="2" t="s">
@@ -11418,10 +11418,10 @@
       <c r="I124" s="2">
         <v>1</v>
       </c>
-      <c r="J124" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K124" s="5" t="s">
+      <c r="J124" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K124" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L124" s="2" t="s">
@@ -11462,10 +11462,10 @@
       <c r="I125" s="2">
         <v>1</v>
       </c>
-      <c r="J125" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K125" s="5" t="s">
+      <c r="J125" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K125" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L125" s="2" t="s">
@@ -11550,10 +11550,10 @@
       <c r="I127" s="2">
         <v>1</v>
       </c>
-      <c r="J127" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K127" s="5" t="s">
+      <c r="J127" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K127" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L127" s="2" t="s">
@@ -11594,10 +11594,10 @@
       <c r="I128" s="2">
         <v>1</v>
       </c>
-      <c r="J128" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K128" s="5" t="s">
+      <c r="J128" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K128" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L128" s="2" t="s">
@@ -11638,10 +11638,10 @@
       <c r="I129" s="2">
         <v>1</v>
       </c>
-      <c r="J129" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K129" s="5" t="s">
+      <c r="J129" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K129" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L129" s="2" t="s">
@@ -11682,10 +11682,10 @@
       <c r="I130" s="2">
         <v>1</v>
       </c>
-      <c r="J130" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K130" s="5" t="s">
+      <c r="J130" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K130" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L130" s="2" t="s">
@@ -11726,10 +11726,10 @@
       <c r="I131" s="2">
         <v>1</v>
       </c>
-      <c r="J131" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K131" s="5" t="s">
+      <c r="J131" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K131" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L131" s="2" t="s">
@@ -11770,10 +11770,10 @@
       <c r="I132" s="2">
         <v>1</v>
       </c>
-      <c r="J132" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K132" s="5" t="s">
+      <c r="J132" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K132" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L132" s="2" t="s">

</xml_diff>

<commit_message>
Correction erreur nom ville
</commit_message>
<xml_diff>
--- a/Jeu d'essai.xlsx
+++ b/Jeu d'essai.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="566" documentId="114_{8D9B191C-2013-4270-87A9-3FB899E57325}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{175A67BF-E76D-446B-87C3-7623B42B2C40}"/>
+  <xr:revisionPtr revIDLastSave="568" documentId="114_{8D9B191C-2013-4270-87A9-3FB899E57325}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{4FDC0E3E-7502-49B1-976B-0A4A3DB3180A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1859" uniqueCount="907">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1859" uniqueCount="906">
   <si>
     <t>NULL</t>
   </si>
@@ -2791,9 +2791,6 @@
   </si>
   <si>
     <t>H4L3P8</t>
-  </si>
-  <si>
-    <t>Monréal</t>
   </si>
   <si>
     <t>2685 Boulevard Pitfield</t>
@@ -3710,7 +3707,7 @@
         <v>792</v>
       </c>
       <c r="E9" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="F9" t="s">
         <v>793</v>
@@ -3775,7 +3772,7 @@
         <v>789</v>
       </c>
       <c r="E10" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="F10" t="s">
         <v>793</v>
@@ -3784,7 +3781,7 @@
         <v>250</v>
       </c>
       <c r="H10" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="I10" t="s">
         <v>252</v>
@@ -3840,7 +3837,7 @@
         <v>790</v>
       </c>
       <c r="E11" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F11" t="s">
         <v>299</v>
@@ -3849,7 +3846,7 @@
         <v>250</v>
       </c>
       <c r="H11" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="I11" t="s">
         <v>252</v>
@@ -5372,7 +5369,7 @@
         <v>312</v>
       </c>
       <c r="G19" t="s">
-        <v>899</v>
+        <v>299</v>
       </c>
       <c r="H19" t="s">
         <v>250</v>
@@ -5740,16 +5737,16 @@
         <v>809</v>
       </c>
       <c r="F26" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="G26" t="s">
-        <v>899</v>
+        <v>299</v>
       </c>
       <c r="H26" t="s">
         <v>250</v>
       </c>
       <c r="I26" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="J26" t="s">
         <v>252</v>

</xml_diff>